<commit_message>
add some descritive text to filter tab
</commit_message>
<xml_diff>
--- a/ExpectedMove/expected_moves.xlsx
+++ b/ExpectedMove/expected_moves.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dallincoons/Projects/expected_move/ExpectedMove/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1838118-381F-7F41-9E5B-ABB1A0B0C3AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83442EC2-C3D2-DD47-8FFD-88CD09F3CA16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42500" yWindow="920" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -305,10 +305,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA68"/>
+  <dimension ref="A1:AA69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -360,20 +360,28 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
-        <v>43913</v>
+        <v>43920</v>
       </c>
       <c r="B2" s="2">
-        <v>43917</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+        <v>43924</v>
+      </c>
+      <c r="C2" s="1">
+        <v>255.7</v>
+      </c>
+      <c r="D2" s="1">
+        <v>263.33</v>
+      </c>
+      <c r="E2" s="1">
+        <v>247.6</v>
+      </c>
+      <c r="F2" s="1">
+        <v>248.89</v>
+      </c>
       <c r="G2" s="1">
-        <v>251.554</v>
+        <v>274.065</v>
       </c>
       <c r="H2" s="1">
-        <v>206.04599999999999</v>
+        <v>232.77500000000001</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -397,28 +405,28 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
-        <v>43906</v>
+        <v>43913</v>
       </c>
       <c r="B3" s="2">
-        <v>43910</v>
+        <v>43917</v>
       </c>
       <c r="C3" s="1">
-        <v>241.18</v>
+        <v>228.19</v>
       </c>
       <c r="D3" s="1">
-        <v>256.89999999999998</v>
+        <v>262.8</v>
       </c>
       <c r="E3" s="1">
-        <v>228.02</v>
+        <v>218.26</v>
       </c>
       <c r="F3" s="1">
-        <v>228.8</v>
+        <v>253.42</v>
       </c>
       <c r="G3" s="1">
-        <v>292.32</v>
+        <v>251.554</v>
       </c>
       <c r="H3" s="1">
-        <v>246.32</v>
+        <v>206.04599999999999</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -442,28 +450,28 @@
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
-        <v>43899</v>
+        <v>43906</v>
       </c>
       <c r="B4" s="2">
-        <v>43903</v>
+        <v>43910</v>
       </c>
       <c r="C4" s="1">
-        <v>275.3</v>
+        <v>241.18</v>
       </c>
       <c r="D4" s="1">
-        <v>288.52</v>
+        <v>256.89999999999998</v>
       </c>
       <c r="E4" s="1">
-        <v>247.68</v>
+        <v>228.02</v>
       </c>
       <c r="F4" s="1">
-        <v>248.11</v>
+        <v>228.8</v>
       </c>
       <c r="G4" s="1">
-        <v>313.53199999999998</v>
+        <v>292.32</v>
       </c>
       <c r="H4" s="1">
-        <v>281.38799999999998</v>
+        <v>246.32</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -487,28 +495,28 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
-        <v>43892</v>
+        <v>43899</v>
       </c>
       <c r="B5" s="2">
-        <v>43896</v>
+        <v>43903</v>
       </c>
       <c r="C5" s="1">
-        <v>298.20999999999998</v>
+        <v>275.3</v>
       </c>
       <c r="D5" s="1">
-        <v>313.83999999999997</v>
+        <v>288.52</v>
       </c>
       <c r="E5" s="1">
-        <v>290.23</v>
+        <v>247.68</v>
       </c>
       <c r="F5" s="1">
-        <v>297.45999999999998</v>
+        <v>248.11</v>
       </c>
       <c r="G5" s="1">
-        <v>314.45999999999998</v>
+        <v>313.53199999999998</v>
       </c>
       <c r="H5" s="1">
-        <v>278.06</v>
+        <v>281.38799999999998</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -532,28 +540,28 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
-        <v>43885</v>
+        <v>43892</v>
       </c>
       <c r="B6" s="2">
-        <v>43889</v>
+        <v>43896</v>
       </c>
       <c r="C6" s="1">
-        <v>323.14</v>
+        <v>298.20999999999998</v>
       </c>
       <c r="D6" s="1">
-        <v>337.06</v>
+        <v>313.83999999999997</v>
       </c>
       <c r="E6" s="1">
-        <v>285.54000000000002</v>
+        <v>290.23</v>
       </c>
       <c r="F6" s="1">
-        <v>296.26</v>
+        <v>297.45999999999998</v>
       </c>
       <c r="G6" s="1">
-        <v>338.75</v>
+        <v>314.45999999999998</v>
       </c>
       <c r="H6" s="1">
-        <v>328.24</v>
+        <v>278.06</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -577,28 +585,28 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
-        <v>43879</v>
+        <v>43885</v>
       </c>
       <c r="B7" s="2">
-        <v>43882</v>
+        <v>43889</v>
       </c>
       <c r="C7" s="1">
-        <v>336.51</v>
+        <v>323.14</v>
       </c>
       <c r="D7" s="1">
-        <v>339.08</v>
+        <v>337.06</v>
       </c>
       <c r="E7" s="1">
-        <v>332.58</v>
+        <v>285.54000000000002</v>
       </c>
       <c r="F7" s="1">
-        <v>333.48</v>
+        <v>296.26</v>
       </c>
       <c r="G7" s="1">
-        <v>341.637</v>
+        <v>338.75</v>
       </c>
       <c r="H7" s="1">
-        <v>333.56299999999999</v>
+        <v>328.24</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -622,28 +630,28 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
-        <v>43871</v>
+        <v>43879</v>
       </c>
       <c r="B8" s="2">
-        <v>43875</v>
+        <v>43882</v>
       </c>
       <c r="C8" s="1">
-        <v>331.23</v>
+        <v>336.51</v>
       </c>
       <c r="D8" s="1">
-        <v>338.12</v>
+        <v>339.08</v>
       </c>
       <c r="E8" s="1">
-        <v>331.19</v>
+        <v>332.58</v>
       </c>
       <c r="F8" s="1">
-        <v>337.6</v>
+        <v>333.48</v>
       </c>
       <c r="G8" s="1">
-        <v>337.32600000000002</v>
+        <v>341.637</v>
       </c>
       <c r="H8" s="1">
-        <v>327.07799999999997</v>
+        <v>333.56299999999999</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -667,28 +675,28 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
-        <v>43864</v>
+        <v>43871</v>
       </c>
       <c r="B9" s="2">
-        <v>43868</v>
+        <v>43875</v>
       </c>
       <c r="C9" s="1">
-        <v>323.35000000000002</v>
+        <v>331.23</v>
       </c>
       <c r="D9" s="1">
-        <v>334.49</v>
+        <v>338.12</v>
       </c>
       <c r="E9" s="1">
-        <v>323.22000000000003</v>
+        <v>331.19</v>
       </c>
       <c r="F9" s="1">
-        <v>332.2</v>
+        <v>337.6</v>
       </c>
       <c r="G9" s="1">
-        <v>327.82</v>
+        <v>337.32600000000002</v>
       </c>
       <c r="H9" s="1">
-        <v>315.64</v>
+        <v>327.07799999999997</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -712,28 +720,28 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
-        <v>43857</v>
+        <v>43864</v>
       </c>
       <c r="B10" s="2">
-        <v>43861</v>
+        <v>43868</v>
       </c>
       <c r="C10" s="1">
-        <v>323.02999999999997</v>
+        <v>323.35000000000002</v>
       </c>
       <c r="D10" s="1">
-        <v>328.63</v>
+        <v>334.49</v>
       </c>
       <c r="E10" s="1">
-        <v>320.73</v>
+        <v>323.22000000000003</v>
       </c>
       <c r="F10" s="1">
-        <v>321.73</v>
+        <v>332.2</v>
       </c>
       <c r="G10" s="1">
-        <v>334.03699999999998</v>
+        <v>327.82</v>
       </c>
       <c r="H10" s="1">
-        <v>323.50400000000002</v>
+        <v>315.64</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -757,28 +765,28 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
-        <v>43851</v>
+        <v>43857</v>
       </c>
       <c r="B11" s="2">
-        <v>43854</v>
+        <v>43861</v>
       </c>
       <c r="C11" s="1">
-        <v>332.44</v>
+        <v>323.02999999999997</v>
       </c>
       <c r="D11" s="1">
-        <v>332.53</v>
+        <v>328.63</v>
       </c>
       <c r="E11" s="1">
-        <v>327.36</v>
+        <v>320.73</v>
       </c>
       <c r="F11" s="1">
-        <v>328.77</v>
+        <v>321.73</v>
       </c>
       <c r="G11" s="1">
-        <v>334.07</v>
+        <v>334.03699999999998</v>
       </c>
       <c r="H11" s="1">
-        <v>329.83</v>
+        <v>323.50400000000002</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -802,28 +810,28 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
-        <v>43843</v>
+        <v>43851</v>
       </c>
       <c r="B12" s="2">
-        <v>43847</v>
+        <v>43854</v>
       </c>
       <c r="C12" s="1">
-        <v>326.39</v>
+        <v>332.44</v>
       </c>
       <c r="D12" s="1">
-        <v>332.18</v>
+        <v>332.53</v>
       </c>
       <c r="E12" s="1">
-        <v>325.92</v>
+        <v>327.36</v>
       </c>
       <c r="F12" s="1">
-        <v>331.95</v>
+        <v>328.77</v>
       </c>
       <c r="G12" s="1">
-        <v>329.14</v>
+        <v>334.07</v>
       </c>
       <c r="H12" s="1">
-        <v>322.27999999999997</v>
+        <v>329.83</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -847,28 +855,28 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
-        <v>43836</v>
+        <v>43843</v>
       </c>
       <c r="B13" s="2">
-        <v>43840</v>
+        <v>43847</v>
       </c>
       <c r="C13" s="1">
-        <v>320.49</v>
+        <v>326.39</v>
       </c>
       <c r="D13" s="1">
-        <v>327.45999999999998</v>
+        <v>332.18</v>
       </c>
       <c r="E13" s="1">
-        <v>325.70999999999998</v>
+        <v>325.92</v>
       </c>
       <c r="F13" s="1">
-        <v>325.70999999999998</v>
+        <v>331.95</v>
       </c>
       <c r="G13" s="1">
-        <v>325.54000000000002</v>
+        <v>329.14</v>
       </c>
       <c r="H13" s="1">
-        <v>319.27999999999997</v>
+        <v>322.27999999999997</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -892,28 +900,28 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
-        <v>43829</v>
+        <v>43836</v>
       </c>
       <c r="B14" s="2">
-        <v>43833</v>
+        <v>43840</v>
       </c>
       <c r="C14" s="1">
-        <v>322.95</v>
+        <v>320.49</v>
       </c>
       <c r="D14" s="1">
-        <v>324.89</v>
+        <v>327.45999999999998</v>
       </c>
       <c r="E14" s="1">
-        <v>320.14999999999998</v>
+        <v>325.70999999999998</v>
       </c>
       <c r="F14" s="1">
-        <v>322.41000000000003</v>
+        <v>325.70999999999998</v>
       </c>
       <c r="G14" s="1">
-        <v>326.23</v>
+        <v>325.54000000000002</v>
       </c>
       <c r="H14" s="1">
-        <v>319.5</v>
+        <v>319.27999999999997</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -937,28 +945,28 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
-        <v>43822</v>
+        <v>43829</v>
       </c>
       <c r="B15" s="2">
-        <v>43826</v>
+        <v>43833</v>
       </c>
       <c r="C15" s="1">
-        <v>321.58999999999997</v>
+        <v>322.95</v>
       </c>
       <c r="D15" s="1">
-        <v>323.8</v>
+        <v>324.89</v>
       </c>
       <c r="E15" s="1">
-        <v>320.89999999999998</v>
+        <v>320.14999999999998</v>
       </c>
       <c r="F15" s="1">
-        <v>322.86</v>
+        <v>322.41000000000003</v>
       </c>
       <c r="G15" s="1">
-        <v>324.20999999999998</v>
+        <v>326.23</v>
       </c>
       <c r="H15" s="1">
-        <v>317.23</v>
+        <v>319.5</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -982,28 +990,28 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
-        <v>43815</v>
+        <v>43822</v>
       </c>
       <c r="B16" s="2">
-        <v>43819</v>
+        <v>43826</v>
       </c>
       <c r="C16" s="1">
-        <v>319.22000000000003</v>
+        <v>321.58999999999997</v>
       </c>
       <c r="D16" s="1">
-        <v>321.97000000000003</v>
+        <v>323.8</v>
       </c>
       <c r="E16" s="1">
-        <v>317.25</v>
+        <v>320.89999999999998</v>
       </c>
       <c r="F16" s="1">
-        <v>320.73</v>
+        <v>322.86</v>
       </c>
       <c r="G16" s="1">
-        <v>320.94</v>
+        <v>324.20999999999998</v>
       </c>
       <c r="H16" s="1">
-        <v>313.70999999999998</v>
+        <v>317.23</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1027,28 +1035,28 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
-        <v>43808</v>
+        <v>43815</v>
       </c>
       <c r="B17" s="2">
-        <v>43812</v>
+        <v>43819</v>
       </c>
       <c r="C17" s="1">
-        <v>314.44</v>
+        <v>319.22000000000003</v>
       </c>
       <c r="D17" s="1">
-        <v>318.67</v>
+        <v>321.97000000000003</v>
       </c>
       <c r="E17" s="1">
-        <v>312.81</v>
+        <v>317.25</v>
       </c>
       <c r="F17" s="1">
-        <v>317.32</v>
+        <v>320.73</v>
       </c>
       <c r="G17" s="1">
-        <v>318.19</v>
+        <v>320.94</v>
       </c>
       <c r="H17" s="1">
-        <v>311.56</v>
+        <v>313.70999999999998</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1072,28 +1080,28 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
-        <v>43801</v>
+        <v>43808</v>
       </c>
       <c r="B18" s="2">
-        <v>43805</v>
+        <v>43812</v>
       </c>
       <c r="C18" s="1">
-        <v>314.58999999999997</v>
+        <v>314.44</v>
       </c>
       <c r="D18" s="1">
-        <v>315.31</v>
+        <v>318.67</v>
       </c>
       <c r="E18" s="1">
-        <v>307.13</v>
+        <v>312.81</v>
       </c>
       <c r="F18" s="1">
-        <v>314.87</v>
+        <v>317.32</v>
       </c>
       <c r="G18" s="1">
-        <v>317.69</v>
+        <v>318.19</v>
       </c>
       <c r="H18" s="1">
-        <v>310.92</v>
+        <v>311.56</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1117,28 +1125,28 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
-        <v>43794</v>
+        <v>43801</v>
       </c>
       <c r="B19" s="2">
-        <v>43798</v>
+        <v>43805</v>
       </c>
       <c r="C19" s="1">
-        <v>311.98</v>
+        <v>314.58999999999997</v>
       </c>
       <c r="D19" s="1">
-        <v>315.48</v>
+        <v>315.31</v>
       </c>
       <c r="E19" s="1">
-        <v>311.98</v>
+        <v>307.13</v>
       </c>
       <c r="F19" s="1">
-        <v>314.31</v>
+        <v>314.87</v>
       </c>
       <c r="G19" s="1">
-        <v>314.56</v>
+        <v>317.69</v>
       </c>
       <c r="H19" s="1">
-        <v>307.39</v>
+        <v>310.92</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1162,28 +1170,28 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
-        <v>43787</v>
+        <v>43794</v>
       </c>
       <c r="B20" s="2">
-        <v>43791</v>
+        <v>43798</v>
       </c>
       <c r="C20" s="1">
-        <v>311.52999999999997</v>
+        <v>311.98</v>
       </c>
       <c r="D20" s="1">
-        <v>312.69</v>
+        <v>315.48</v>
       </c>
       <c r="E20" s="1">
-        <v>309.06</v>
+        <v>311.98</v>
       </c>
       <c r="F20" s="1">
-        <v>310.95999999999998</v>
+        <v>314.31</v>
       </c>
       <c r="G20" s="1">
-        <v>315.3</v>
+        <v>314.56</v>
       </c>
       <c r="H20" s="1">
-        <v>308.25</v>
+        <v>307.39</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1207,28 +1215,28 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
-        <v>43780</v>
+        <v>43787</v>
       </c>
       <c r="B21" s="2">
-        <v>43784</v>
+        <v>43791</v>
       </c>
       <c r="C21" s="1">
-        <v>307.42</v>
+        <v>311.52999999999997</v>
       </c>
       <c r="D21" s="1">
-        <v>311.83999999999997</v>
+        <v>312.69</v>
       </c>
       <c r="E21" s="1">
-        <v>307.27</v>
+        <v>309.06</v>
       </c>
       <c r="F21" s="1">
-        <v>311.79000000000002</v>
+        <v>310.95999999999998</v>
       </c>
       <c r="G21" s="1">
-        <v>312.52</v>
+        <v>315.3</v>
       </c>
       <c r="H21" s="1">
-        <v>305.36</v>
+        <v>308.25</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1252,28 +1260,28 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
-        <v>43773</v>
+        <v>43780</v>
       </c>
       <c r="B22" s="2">
-        <v>43777</v>
+        <v>43784</v>
       </c>
       <c r="C22" s="1">
-        <v>307.85000000000002</v>
+        <v>307.42</v>
       </c>
       <c r="D22" s="1">
-        <v>309.64999999999998</v>
+        <v>311.83999999999997</v>
       </c>
       <c r="E22" s="1">
-        <v>306.06</v>
+        <v>307.27</v>
       </c>
       <c r="F22" s="1">
-        <v>308.94</v>
+        <v>311.79000000000002</v>
       </c>
       <c r="G22" s="1">
-        <v>309.85000000000002</v>
+        <v>312.52</v>
       </c>
       <c r="H22" s="1">
-        <v>302.44</v>
+        <v>305.36</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1297,28 +1305,28 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
-        <v>43766</v>
+        <v>43773</v>
       </c>
       <c r="B23" s="2">
-        <v>43770</v>
+        <v>43777</v>
       </c>
       <c r="C23" s="1">
-        <v>302.94</v>
+        <v>307.85000000000002</v>
       </c>
       <c r="D23" s="1">
-        <v>306.19</v>
+        <v>309.64999999999998</v>
       </c>
       <c r="E23" s="1">
-        <v>301.73</v>
+        <v>306.06</v>
       </c>
       <c r="F23" s="1">
-        <v>306.14</v>
+        <v>308.94</v>
       </c>
       <c r="G23" s="1">
-        <v>305.2</v>
+        <v>309.85000000000002</v>
       </c>
       <c r="H23" s="1">
-        <v>298.01</v>
+        <v>302.44</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1342,28 +1350,28 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
-        <v>43759</v>
+        <v>43766</v>
       </c>
       <c r="B24" s="2">
-        <v>43763</v>
+        <v>43770</v>
       </c>
       <c r="C24" s="1">
-        <v>299.42</v>
+        <v>302.94</v>
       </c>
       <c r="D24" s="1">
-        <v>302.2</v>
+        <v>306.19</v>
       </c>
       <c r="E24" s="1">
-        <v>298.5</v>
+        <v>301.73</v>
       </c>
       <c r="F24" s="1">
-        <v>301.60000000000002</v>
+        <v>306.14</v>
       </c>
       <c r="G24" s="1">
-        <v>301.77999999999997</v>
+        <v>305.2</v>
       </c>
       <c r="H24" s="1">
-        <v>294.14999999999998</v>
+        <v>298.01</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1387,28 +1395,28 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
-        <v>43752</v>
+        <v>43759</v>
       </c>
       <c r="B25" s="2">
-        <v>43756</v>
+        <v>43763</v>
       </c>
       <c r="C25" s="1">
-        <v>295.93</v>
+        <v>299.42</v>
       </c>
       <c r="D25" s="1">
-        <v>300.24</v>
+        <v>302.2</v>
       </c>
       <c r="E25" s="1">
-        <v>295.57</v>
+        <v>298.5</v>
       </c>
       <c r="F25" s="1">
-        <v>297.97000000000003</v>
+        <v>301.60000000000002</v>
       </c>
       <c r="G25" s="1">
-        <v>300.29000000000002</v>
+        <v>301.77999999999997</v>
       </c>
       <c r="H25" s="1">
-        <v>292.26</v>
+        <v>294.14999999999998</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1432,28 +1440,28 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
-        <v>43745</v>
+        <v>43752</v>
       </c>
       <c r="B26" s="2">
-        <v>43749</v>
+        <v>43756</v>
       </c>
       <c r="C26" s="1">
-        <v>293.47000000000003</v>
+        <v>295.93</v>
       </c>
       <c r="D26" s="1">
-        <v>298.74</v>
+        <v>300.24</v>
       </c>
       <c r="E26" s="1">
-        <v>288.49</v>
+        <v>295.57</v>
       </c>
       <c r="F26" s="1">
-        <v>296.27999999999997</v>
+        <v>297.97000000000003</v>
       </c>
       <c r="G26" s="1">
-        <v>298.93</v>
+        <v>300.29000000000002</v>
       </c>
       <c r="H26" s="1">
-        <v>289.74</v>
+        <v>292.26</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1477,28 +1485,28 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
-        <v>43738</v>
+        <v>43745</v>
       </c>
       <c r="B27" s="2">
-        <v>43742</v>
+        <v>43749</v>
       </c>
       <c r="C27" s="1">
-        <v>295.97000000000003</v>
+        <v>293.47000000000003</v>
       </c>
       <c r="D27" s="1">
-        <v>298.45999999999998</v>
+        <v>298.74</v>
       </c>
       <c r="E27" s="1">
-        <v>284.82</v>
+        <v>288.49</v>
       </c>
       <c r="F27" s="1">
-        <v>294.35000000000002</v>
+        <v>296.27999999999997</v>
       </c>
       <c r="G27" s="1">
-        <v>300.01</v>
+        <v>298.93</v>
       </c>
       <c r="H27" s="1">
-        <v>290.77999999999997</v>
+        <v>289.74</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1522,28 +1530,28 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
-        <v>43731</v>
+        <v>43738</v>
       </c>
       <c r="B28" s="2">
-        <v>43735</v>
+        <v>43742</v>
       </c>
       <c r="C28" s="1">
-        <v>297.55</v>
+        <v>295.97000000000003</v>
       </c>
       <c r="D28" s="1">
-        <v>299.83999999999997</v>
+        <v>298.45999999999998</v>
       </c>
       <c r="E28" s="1">
-        <v>293.69</v>
+        <v>284.82</v>
       </c>
       <c r="F28" s="1">
-        <v>295.39999999999998</v>
+        <v>294.35000000000002</v>
       </c>
       <c r="G28" s="1">
-        <v>302.43</v>
+        <v>300.01</v>
       </c>
       <c r="H28" s="1">
-        <v>294.13</v>
+        <v>290.77999999999997</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1567,28 +1575,28 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
-        <v>43724</v>
+        <v>43731</v>
       </c>
       <c r="B29" s="2">
-        <v>43728</v>
+        <v>43735</v>
       </c>
       <c r="C29" s="1">
+        <v>297.55</v>
+      </c>
+      <c r="D29" s="1">
         <v>299.83999999999997</v>
       </c>
-      <c r="D29" s="1">
-        <v>302.63</v>
-      </c>
       <c r="E29" s="1">
-        <v>297.41000000000003</v>
+        <v>293.69</v>
       </c>
       <c r="F29" s="1">
-        <v>298.27999999999997</v>
+        <v>295.39999999999998</v>
       </c>
       <c r="G29" s="1">
-        <v>304.77999999999997</v>
+        <v>302.43</v>
       </c>
       <c r="H29" s="1">
-        <v>297.39999999999998</v>
+        <v>294.13</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1612,28 +1620,28 @@
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
-        <v>43717</v>
+        <v>43724</v>
       </c>
       <c r="B30" s="2">
-        <v>43721</v>
+        <v>43728</v>
       </c>
       <c r="C30" s="1">
-        <v>299.14</v>
+        <v>299.83999999999997</v>
       </c>
       <c r="D30" s="1">
-        <v>302.45999999999998</v>
+        <v>302.63</v>
       </c>
       <c r="E30" s="1">
-        <v>295.97000000000003</v>
+        <v>297.41000000000003</v>
       </c>
       <c r="F30" s="1">
-        <v>301.08999999999997</v>
+        <v>298.27999999999997</v>
       </c>
       <c r="G30" s="1">
-        <v>302.2</v>
+        <v>304.77999999999997</v>
       </c>
       <c r="H30" s="1">
-        <v>293.89999999999998</v>
+        <v>297.39999999999998</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -1657,28 +1665,28 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
-        <v>43711</v>
+        <v>43717</v>
       </c>
       <c r="B31" s="2">
-        <v>43714</v>
+        <v>43721</v>
       </c>
       <c r="C31" s="1">
-        <v>290.57</v>
+        <v>299.14</v>
       </c>
       <c r="D31" s="1">
-        <v>298.83</v>
+        <v>302.45999999999998</v>
       </c>
       <c r="E31" s="1">
-        <v>289.27</v>
+        <v>295.97000000000003</v>
       </c>
       <c r="F31" s="1">
-        <v>298.05</v>
+        <v>301.08999999999997</v>
       </c>
       <c r="G31" s="1">
-        <v>297.49</v>
+        <v>302.2</v>
       </c>
       <c r="H31" s="1">
-        <v>287.39</v>
+        <v>293.89999999999998</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1702,28 +1710,28 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
-        <v>43703</v>
+        <v>43711</v>
       </c>
       <c r="B32" s="2">
-        <v>43707</v>
+        <v>43714</v>
       </c>
       <c r="C32" s="1">
-        <v>287.27</v>
+        <v>290.57</v>
       </c>
       <c r="D32" s="1">
-        <v>294.24</v>
+        <v>298.83</v>
       </c>
       <c r="E32" s="1">
-        <v>285.25</v>
+        <v>289.27</v>
       </c>
       <c r="F32" s="1">
-        <v>292.45</v>
+        <v>298.05</v>
       </c>
       <c r="G32" s="1">
-        <v>290.10000000000002</v>
+        <v>297.49</v>
       </c>
       <c r="H32" s="1">
-        <v>279.60000000000002</v>
+        <v>287.39</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1747,28 +1755,28 @@
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="B33" s="2">
-        <v>43700</v>
+        <v>43707</v>
       </c>
       <c r="C33" s="1">
-        <v>292.19</v>
+        <v>287.27</v>
       </c>
       <c r="D33" s="1">
-        <v>293.93</v>
+        <v>294.24</v>
       </c>
       <c r="E33" s="1">
-        <v>283.47000000000003</v>
+        <v>285.25</v>
       </c>
       <c r="F33" s="1">
-        <v>284.85000000000002</v>
+        <v>292.45</v>
       </c>
       <c r="G33" s="1">
-        <v>293.75</v>
+        <v>290.10000000000002</v>
       </c>
       <c r="H33" s="1">
-        <v>283.94</v>
+        <v>279.60000000000002</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1792,28 +1800,28 @@
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
-        <v>43689</v>
+        <v>43696</v>
       </c>
       <c r="B34" s="2">
-        <v>43693</v>
+        <v>43700</v>
       </c>
       <c r="C34" s="1">
-        <v>289.95999999999998</v>
+        <v>292.19</v>
       </c>
       <c r="D34" s="1">
-        <v>294.14999999999998</v>
+        <v>293.93</v>
       </c>
       <c r="E34" s="1">
-        <v>282.39</v>
+        <v>283.47000000000003</v>
       </c>
       <c r="F34" s="1">
-        <v>288.85000000000002</v>
+        <v>284.85000000000002</v>
       </c>
       <c r="G34" s="1">
-        <v>296.31</v>
+        <v>293.75</v>
       </c>
       <c r="H34" s="1">
-        <v>286.95</v>
+        <v>283.94</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1837,28 +1845,28 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
-        <v>43682</v>
+        <v>43689</v>
       </c>
       <c r="B35" s="2">
-        <v>43686</v>
+        <v>43693</v>
       </c>
       <c r="C35" s="1">
-        <v>288.08999999999997</v>
+        <v>289.95999999999998</v>
       </c>
       <c r="D35" s="1">
-        <v>293.62</v>
+        <v>294.14999999999998</v>
       </c>
       <c r="E35" s="1">
-        <v>281.72000000000003</v>
+        <v>282.39</v>
       </c>
       <c r="F35" s="1">
-        <v>291.62</v>
+        <v>288.85000000000002</v>
       </c>
       <c r="G35" s="1">
-        <v>296.85000000000002</v>
+        <v>296.31</v>
       </c>
       <c r="H35" s="1">
-        <v>288.33</v>
+        <v>286.95</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -1882,28 +1890,28 @@
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
-        <v>43675</v>
+        <v>43682</v>
       </c>
       <c r="B36" s="2">
-        <v>43679</v>
+        <v>43686</v>
       </c>
       <c r="C36" s="1">
-        <v>301.88</v>
+        <v>288.08999999999997</v>
       </c>
       <c r="D36" s="1">
-        <v>301.93</v>
+        <v>293.62</v>
       </c>
       <c r="E36" s="1">
-        <v>290.89999999999998</v>
+        <v>281.72000000000003</v>
       </c>
       <c r="F36" s="1">
-        <v>292.62</v>
+        <v>291.62</v>
       </c>
       <c r="G36" s="1">
-        <v>305.18</v>
+        <v>296.85000000000002</v>
       </c>
       <c r="H36" s="1">
-        <v>298.86</v>
+        <v>288.33</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -1927,28 +1935,28 @@
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
-        <v>43668</v>
+        <v>43675</v>
       </c>
       <c r="B37" s="2">
-        <v>43672</v>
+        <v>43679</v>
       </c>
       <c r="C37" s="1">
-        <v>297.61</v>
+        <v>301.88</v>
       </c>
       <c r="D37" s="1">
-        <v>302.23</v>
+        <v>301.93</v>
       </c>
       <c r="E37" s="1">
-        <v>297.04000000000002</v>
+        <v>290.89999999999998</v>
       </c>
       <c r="F37" s="1">
-        <v>302.01</v>
+        <v>292.62</v>
       </c>
       <c r="G37" s="1">
-        <v>301.06</v>
+        <v>305.18</v>
       </c>
       <c r="H37" s="1">
-        <v>293.26</v>
+        <v>298.86</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -1972,28 +1980,28 @@
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
-        <v>43661</v>
+        <v>43668</v>
       </c>
       <c r="B38" s="2">
-        <v>43665</v>
+        <v>43672</v>
       </c>
       <c r="C38" s="1">
-        <v>301.13</v>
+        <v>297.61</v>
       </c>
       <c r="D38" s="1">
-        <v>301.13</v>
+        <v>302.23</v>
       </c>
       <c r="E38" s="1">
-        <v>296.7</v>
+        <v>297.04000000000002</v>
       </c>
       <c r="F38" s="1">
-        <v>297.17</v>
+        <v>302.01</v>
       </c>
       <c r="G38" s="1">
-        <v>303.86</v>
+        <v>301.06</v>
       </c>
       <c r="H38" s="1">
-        <v>297.49</v>
+        <v>293.26</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2017,28 +2025,28 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
-        <v>43654</v>
+        <v>43661</v>
       </c>
       <c r="B39" s="2">
-        <v>43658</v>
+        <v>43665</v>
       </c>
       <c r="C39" s="1">
-        <v>297.01</v>
+        <v>301.13</v>
       </c>
       <c r="D39" s="1">
-        <v>300.73</v>
+        <v>301.13</v>
       </c>
       <c r="E39" s="1">
-        <v>295.48</v>
+        <v>296.7</v>
       </c>
       <c r="F39" s="1">
-        <v>300.64999999999998</v>
+        <v>297.17</v>
       </c>
       <c r="G39" s="1">
-        <v>301.94</v>
+        <v>303.86</v>
       </c>
       <c r="H39" s="1">
-        <v>295</v>
+        <v>297.49</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -2062,28 +2070,28 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
-        <v>43647</v>
+        <v>43654</v>
       </c>
       <c r="B40" s="2">
-        <v>43651</v>
+        <v>43658</v>
       </c>
       <c r="C40" s="1">
-        <v>296.68</v>
+        <v>297.01</v>
       </c>
       <c r="D40" s="1">
-        <v>298.82</v>
+        <v>300.73</v>
       </c>
       <c r="E40" s="1">
-        <v>294.33</v>
+        <v>295.48</v>
       </c>
       <c r="F40" s="1">
-        <v>298.45999999999998</v>
+        <v>300.64999999999998</v>
       </c>
       <c r="G40" s="1">
-        <v>296.95999999999998</v>
+        <v>301.94</v>
       </c>
       <c r="H40" s="1">
-        <v>289.04000000000002</v>
+        <v>295</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -2107,28 +2115,28 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
-        <v>43640</v>
+        <v>43647</v>
       </c>
       <c r="B41" s="2">
-        <v>43644</v>
+        <v>43651</v>
       </c>
       <c r="C41" s="1">
-        <v>294.23</v>
+        <v>296.68</v>
       </c>
       <c r="D41" s="1">
-        <v>294.58</v>
+        <v>298.82</v>
       </c>
       <c r="E41" s="1">
-        <v>290.35000000000002</v>
+        <v>294.33</v>
       </c>
       <c r="F41" s="1">
-        <v>293</v>
+        <v>298.45999999999998</v>
       </c>
       <c r="G41" s="1">
-        <v>298.08999999999997</v>
+        <v>296.95999999999998</v>
       </c>
       <c r="H41" s="1">
-        <v>289.87</v>
+        <v>289.04000000000002</v>
       </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -2152,28 +2160,28 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
-        <v>43633</v>
+        <v>43640</v>
       </c>
       <c r="B42" s="2">
-        <v>43637</v>
+        <v>43644</v>
       </c>
       <c r="C42" s="1">
-        <v>289.52</v>
+        <v>294.23</v>
       </c>
       <c r="D42" s="1">
-        <v>296.31</v>
+        <v>294.58</v>
       </c>
       <c r="E42" s="1">
-        <v>289.18</v>
+        <v>290.35000000000002</v>
       </c>
       <c r="F42" s="1">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G42" s="1">
-        <v>293.19</v>
+        <v>298.08999999999997</v>
       </c>
       <c r="H42" s="1">
-        <v>285.33999999999997</v>
+        <v>289.87</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -2197,28 +2205,28 @@
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
-        <v>43626</v>
+        <v>43633</v>
       </c>
       <c r="B43" s="2">
-        <v>43630</v>
+        <v>43637</v>
       </c>
       <c r="C43" s="1">
-        <v>289.37</v>
+        <v>289.52</v>
       </c>
       <c r="D43" s="1">
-        <v>291.39999999999998</v>
+        <v>296.31</v>
       </c>
       <c r="E43" s="1">
-        <v>287.82</v>
+        <v>289.18</v>
       </c>
       <c r="F43" s="1">
-        <v>289.26</v>
+        <v>294</v>
       </c>
       <c r="G43" s="1">
-        <v>291.85000000000002</v>
+        <v>293.19</v>
       </c>
       <c r="H43" s="1">
-        <v>283.44</v>
+        <v>285.33999999999997</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -2242,28 +2250,28 @@
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
-        <v>43619</v>
+        <v>43626</v>
       </c>
       <c r="B44" s="2">
-        <v>43623</v>
+        <v>43630</v>
       </c>
       <c r="C44" s="1">
-        <v>275.31</v>
+        <v>289.37</v>
       </c>
       <c r="D44" s="1">
-        <v>288.85000000000002</v>
+        <v>291.39999999999998</v>
       </c>
       <c r="E44" s="1">
-        <v>273.08999999999997</v>
+        <v>287.82</v>
       </c>
       <c r="F44" s="1">
-        <v>287.64999999999998</v>
+        <v>289.26</v>
       </c>
       <c r="G44" s="1">
-        <v>279.93</v>
+        <v>291.85000000000002</v>
       </c>
       <c r="H44" s="1">
-        <v>270.63</v>
+        <v>283.44</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -2287,28 +2295,28 @@
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
-        <v>43613</v>
+        <v>43619</v>
       </c>
       <c r="B45" s="2">
-        <v>43616</v>
+        <v>43623</v>
       </c>
       <c r="C45" s="1">
-        <v>283.08999999999997</v>
+        <v>275.31</v>
       </c>
       <c r="D45" s="1">
-        <v>284.14999999999998</v>
+        <v>288.85000000000002</v>
       </c>
       <c r="E45" s="1">
-        <v>275.24</v>
+        <v>273.08999999999997</v>
       </c>
       <c r="F45" s="1">
-        <v>275.27</v>
+        <v>287.64999999999998</v>
       </c>
       <c r="G45" s="1">
-        <v>286.89999999999998</v>
+        <v>279.93</v>
       </c>
       <c r="H45" s="1">
-        <v>278.63</v>
+        <v>270.63</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -2332,28 +2340,28 @@
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
-        <v>43605</v>
+        <v>43613</v>
       </c>
       <c r="B46" s="2">
-        <v>43609</v>
+        <v>43616</v>
       </c>
       <c r="C46" s="1">
-        <v>284.06</v>
+        <v>283.08999999999997</v>
       </c>
       <c r="D46" s="1">
-        <v>286.93</v>
+        <v>284.14999999999998</v>
       </c>
       <c r="E46" s="1">
-        <v>280.57</v>
+        <v>275.24</v>
       </c>
       <c r="F46" s="1">
-        <v>282.77999999999997</v>
+        <v>275.27</v>
       </c>
       <c r="G46" s="1">
-        <v>290</v>
+        <v>286.89999999999998</v>
       </c>
       <c r="H46" s="1">
-        <v>281.63</v>
+        <v>278.63</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -2377,28 +2385,28 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
-        <v>43598</v>
+        <v>43605</v>
       </c>
       <c r="B47" s="2">
-        <v>43602</v>
+        <v>43609</v>
       </c>
       <c r="C47" s="1">
-        <v>282.42</v>
+        <v>284.06</v>
       </c>
       <c r="D47" s="1">
-        <v>289.20999999999998</v>
+        <v>286.93</v>
       </c>
       <c r="E47" s="1">
-        <v>279.93</v>
+        <v>280.57</v>
       </c>
       <c r="F47" s="1">
-        <v>285.83999999999997</v>
+        <v>282.77999999999997</v>
       </c>
       <c r="G47" s="1">
-        <v>292.32</v>
+        <v>290</v>
       </c>
       <c r="H47" s="1">
-        <v>283.8</v>
+        <v>281.63</v>
       </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
@@ -2422,28 +2430,28 @@
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
-        <v>43591</v>
+        <v>43598</v>
       </c>
       <c r="B48" s="2">
-        <v>43595</v>
+        <v>43602</v>
       </c>
       <c r="C48" s="1">
-        <v>289.25</v>
+        <v>282.42</v>
       </c>
       <c r="D48" s="1">
-        <v>293.31</v>
+        <v>289.20999999999998</v>
       </c>
       <c r="E48" s="1">
-        <v>282.3</v>
+        <v>279.93</v>
       </c>
       <c r="F48" s="1">
-        <v>288.10000000000002</v>
+        <v>285.83999999999997</v>
       </c>
       <c r="G48" s="1">
-        <v>297.17</v>
+        <v>292.32</v>
       </c>
       <c r="H48" s="1">
-        <v>290.87</v>
+        <v>283.8</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -2467,28 +2475,28 @@
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
-        <v>43584</v>
+        <v>43591</v>
       </c>
       <c r="B49" s="2">
-        <v>43588</v>
+        <v>43595</v>
       </c>
       <c r="C49" s="1">
-        <v>293.51</v>
+        <v>289.25</v>
       </c>
       <c r="D49" s="1">
-        <v>294.95</v>
+        <v>293.31</v>
       </c>
       <c r="E49" s="1">
-        <v>289.52</v>
+        <v>282.3</v>
       </c>
       <c r="F49" s="1">
-        <v>294.02999999999997</v>
+        <v>288.10000000000002</v>
       </c>
       <c r="G49" s="1">
-        <v>296.5</v>
+        <v>297.17</v>
       </c>
       <c r="H49" s="1">
-        <v>290.25</v>
+        <v>290.87</v>
       </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
@@ -2512,28 +2520,28 @@
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
-        <v>43577</v>
+        <v>43584</v>
       </c>
       <c r="B50" s="2">
-        <v>43581</v>
+        <v>43588</v>
       </c>
       <c r="C50" s="1">
-        <v>289.17</v>
+        <v>293.51</v>
       </c>
       <c r="D50" s="1">
-        <v>293.49</v>
+        <v>294.95</v>
       </c>
       <c r="E50" s="1">
-        <v>289.07</v>
+        <v>289.52</v>
       </c>
       <c r="F50" s="1">
-        <v>293.41000000000003</v>
+        <v>294.02999999999997</v>
       </c>
       <c r="G50" s="1">
-        <v>293.19</v>
+        <v>296.5</v>
       </c>
       <c r="H50" s="1">
-        <v>286.85000000000002</v>
+        <v>290.25</v>
       </c>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
@@ -2557,28 +2565,28 @@
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
-        <v>43570</v>
+        <v>43577</v>
       </c>
       <c r="B51" s="2">
-        <v>43574</v>
+        <v>43581</v>
       </c>
       <c r="C51" s="1">
-        <v>290.24</v>
+        <v>289.17</v>
       </c>
       <c r="D51" s="1">
-        <v>291.43</v>
+        <v>293.49</v>
       </c>
       <c r="E51" s="1">
-        <v>288.66000000000003</v>
+        <v>289.07</v>
       </c>
       <c r="F51" s="1">
-        <v>290.02</v>
+        <v>293.41000000000003</v>
       </c>
       <c r="G51" s="1">
         <v>293.19</v>
       </c>
       <c r="H51" s="1">
-        <v>287.14</v>
+        <v>286.85000000000002</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
@@ -2602,28 +2610,28 @@
     </row>
     <row r="52" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2">
-        <v>43563</v>
+        <v>43570</v>
       </c>
       <c r="B52" s="2">
-        <v>43567</v>
+        <v>43574</v>
       </c>
       <c r="C52" s="1">
-        <v>288.10000000000002</v>
+        <v>290.24</v>
       </c>
       <c r="D52" s="1">
-        <v>290.47000000000003</v>
+        <v>291.43</v>
       </c>
       <c r="E52" s="1">
-        <v>286.7</v>
+        <v>288.66000000000003</v>
       </c>
       <c r="F52" s="1">
-        <v>290.16000000000003</v>
+        <v>290.02</v>
       </c>
       <c r="G52" s="1">
-        <v>291.89999999999998</v>
+        <v>293.19</v>
       </c>
       <c r="H52" s="1">
-        <v>285.2</v>
+        <v>287.14</v>
       </c>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
@@ -2647,28 +2655,28 @@
     </row>
     <row r="53" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="2">
-        <v>43556</v>
+        <v>43563</v>
       </c>
       <c r="B53" s="2">
-        <v>43560</v>
+        <v>43567</v>
       </c>
       <c r="C53" s="1">
-        <v>284.7</v>
+        <v>288.10000000000002</v>
       </c>
       <c r="D53" s="1">
-        <v>288.63</v>
+        <v>290.47000000000003</v>
       </c>
       <c r="E53" s="1">
-        <v>284.39999999999998</v>
+        <v>286.7</v>
       </c>
       <c r="F53" s="1">
-        <v>288.57</v>
+        <v>290.16000000000003</v>
       </c>
       <c r="G53" s="1">
-        <v>286.06</v>
+        <v>291.89999999999998</v>
       </c>
       <c r="H53" s="1">
-        <v>278.93</v>
+        <v>285.2</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
@@ -2692,28 +2700,28 @@
     </row>
     <row r="54" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="2">
-        <v>43549</v>
+        <v>43556</v>
       </c>
       <c r="B54" s="2">
-        <v>43553</v>
+        <v>43560</v>
       </c>
       <c r="C54" s="1">
-        <v>278.87</v>
+        <v>284.7</v>
       </c>
       <c r="D54" s="1">
-        <v>282.83999999999997</v>
+        <v>288.63</v>
       </c>
       <c r="E54" s="1">
-        <v>277.64</v>
+        <v>284.39999999999998</v>
       </c>
       <c r="F54" s="1">
-        <v>282.48</v>
+        <v>288.57</v>
       </c>
       <c r="G54" s="1">
-        <v>283.33</v>
+        <v>286.06</v>
       </c>
       <c r="H54" s="1">
-        <v>275.11</v>
+        <v>278.93</v>
       </c>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
@@ -2737,28 +2745,28 @@
     </row>
     <row r="55" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="2">
-        <v>43542</v>
+        <v>43549</v>
       </c>
       <c r="B55" s="2">
-        <v>43546</v>
+        <v>43553</v>
       </c>
       <c r="C55" s="1">
-        <v>281.55</v>
+        <v>278.87</v>
       </c>
       <c r="D55" s="1">
-        <v>285.18</v>
+        <v>282.83999999999997</v>
       </c>
       <c r="E55" s="1">
-        <v>279.18</v>
+        <v>277.64</v>
       </c>
       <c r="F55" s="1">
-        <v>279.25</v>
+        <v>282.48</v>
       </c>
       <c r="G55" s="1">
-        <v>284.55</v>
+        <v>283.33</v>
       </c>
       <c r="H55" s="1">
-        <v>278.14</v>
+        <v>275.11</v>
       </c>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
@@ -2782,28 +2790,28 @@
     </row>
     <row r="56" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="2">
-        <v>43535</v>
+        <v>43542</v>
       </c>
       <c r="B56" s="2">
-        <v>43539</v>
+        <v>43546</v>
       </c>
       <c r="C56" s="1">
-        <v>275.26</v>
+        <v>281.55</v>
       </c>
       <c r="D56" s="1">
-        <v>282.38</v>
+        <v>285.18</v>
       </c>
       <c r="E56" s="1">
-        <v>275.23</v>
+        <v>279.18</v>
       </c>
       <c r="F56" s="1">
-        <v>281.31</v>
+        <v>279.25</v>
       </c>
       <c r="G56" s="1">
-        <v>278.36</v>
+        <v>284.55</v>
       </c>
       <c r="H56" s="1">
-        <v>270.58</v>
+        <v>278.14</v>
       </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
@@ -2827,28 +2835,28 @@
     </row>
     <row r="57" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="2">
-        <v>43528</v>
+        <v>43535</v>
       </c>
       <c r="B57" s="2">
-        <v>43532</v>
+        <v>43539</v>
       </c>
       <c r="C57" s="1">
-        <v>281.60000000000002</v>
+        <v>275.26</v>
       </c>
       <c r="D57" s="1">
-        <v>281.87</v>
+        <v>282.38</v>
       </c>
       <c r="E57" s="1">
-        <v>272.42</v>
+        <v>275.23</v>
       </c>
       <c r="F57" s="1">
-        <v>274.45999999999998</v>
+        <v>281.31</v>
       </c>
       <c r="G57" s="1">
-        <v>283.89999999999998</v>
+        <v>278.36</v>
       </c>
       <c r="H57" s="1">
-        <v>276.92</v>
+        <v>270.58</v>
       </c>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
@@ -2872,28 +2880,28 @@
     </row>
     <row r="58" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="2">
-        <v>43521</v>
+        <v>43528</v>
       </c>
       <c r="B58" s="2">
-        <v>43525</v>
+        <v>43532</v>
       </c>
       <c r="C58" s="1">
-        <v>280.73</v>
+        <v>281.60000000000002</v>
       </c>
       <c r="D58" s="1">
-        <v>281.31</v>
+        <v>281.87</v>
       </c>
       <c r="E58" s="1">
-        <v>277.48</v>
+        <v>272.42</v>
       </c>
       <c r="F58" s="1">
-        <v>280.42</v>
+        <v>274.45999999999998</v>
       </c>
       <c r="G58" s="1">
-        <v>282.52</v>
+        <v>283.89999999999998</v>
       </c>
       <c r="H58" s="1">
-        <v>275.62</v>
+        <v>276.92</v>
       </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
@@ -2917,28 +2925,28 @@
     </row>
     <row r="59" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="2">
-        <v>43515</v>
+        <v>43521</v>
       </c>
       <c r="B59" s="2">
-        <v>43518</v>
+        <v>43525</v>
       </c>
       <c r="C59" s="1">
-        <v>276.48</v>
+        <v>280.73</v>
       </c>
       <c r="D59" s="1">
-        <v>279.36</v>
+        <v>281.31</v>
       </c>
       <c r="E59" s="1">
-        <v>276.35000000000002</v>
+        <v>277.48</v>
       </c>
       <c r="F59" s="1">
-        <v>279.14</v>
+        <v>280.42</v>
       </c>
       <c r="G59" s="1">
-        <v>281.24</v>
+        <v>282.52</v>
       </c>
       <c r="H59" s="1">
-        <v>273.45999999999998</v>
+        <v>275.62</v>
       </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
@@ -2962,28 +2970,28 @@
     </row>
     <row r="60" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="2">
-        <v>43507</v>
+        <v>43515</v>
       </c>
       <c r="B60" s="2">
-        <v>43511</v>
+        <v>43518</v>
       </c>
       <c r="C60" s="1">
-        <v>271.2</v>
+        <v>276.48</v>
       </c>
       <c r="D60" s="1">
-        <v>277.41000000000003</v>
+        <v>279.36</v>
       </c>
       <c r="E60" s="1">
-        <v>270.02999999999997</v>
+        <v>276.35000000000002</v>
       </c>
       <c r="F60" s="1">
-        <v>277.37</v>
+        <v>279.14</v>
       </c>
       <c r="G60" s="1">
-        <v>274.39</v>
+        <v>281.24</v>
       </c>
       <c r="H60" s="1">
-        <v>266.54000000000002</v>
+        <v>273.45999999999998</v>
       </c>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
@@ -3007,28 +3015,28 @@
     </row>
     <row r="61" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="2">
-        <v>43500</v>
+        <v>43507</v>
       </c>
       <c r="B61" s="2">
-        <v>43504</v>
+        <v>43511</v>
       </c>
       <c r="C61" s="1">
-        <v>270.11</v>
+        <v>271.2</v>
       </c>
       <c r="D61" s="1">
-        <v>273.44</v>
+        <v>277.41000000000003</v>
       </c>
       <c r="E61" s="1">
-        <v>267.83</v>
+        <v>270.02999999999997</v>
       </c>
       <c r="F61" s="1">
-        <v>270.47000000000003</v>
+        <v>277.37</v>
       </c>
       <c r="G61" s="1">
-        <v>273.17</v>
+        <v>274.39</v>
       </c>
       <c r="H61" s="1">
-        <v>266.98</v>
+        <v>266.54000000000002</v>
       </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
@@ -3052,28 +3060,28 @@
     </row>
     <row r="62" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="2">
-        <v>43493</v>
+        <v>43500</v>
       </c>
       <c r="B62" s="2">
-        <v>43497</v>
+        <v>43504</v>
       </c>
       <c r="C62" s="1">
-        <v>263.39</v>
+        <v>270.11</v>
       </c>
       <c r="D62" s="1">
-        <v>271.2</v>
+        <v>273.44</v>
       </c>
       <c r="E62" s="1">
-        <v>261.79000000000002</v>
+        <v>267.83</v>
       </c>
       <c r="F62" s="1">
-        <v>270.06</v>
+        <v>270.47000000000003</v>
       </c>
       <c r="G62" s="1">
-        <v>269.27999999999997</v>
+        <v>273.17</v>
       </c>
       <c r="H62" s="1">
-        <v>262.08</v>
+        <v>266.98</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
@@ -3097,28 +3105,28 @@
     </row>
     <row r="63" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="2">
-        <v>43487</v>
+        <v>43493</v>
       </c>
       <c r="B63" s="2">
-        <v>43490</v>
+        <v>43497</v>
       </c>
       <c r="C63" s="1">
-        <v>264.82</v>
+        <v>263.39</v>
       </c>
       <c r="D63" s="1">
-        <v>266.7</v>
+        <v>271.2</v>
       </c>
       <c r="E63" s="1">
-        <v>260.66000000000003</v>
+        <v>261.79000000000002</v>
       </c>
       <c r="F63" s="1">
-        <v>265.77999999999997</v>
+        <v>270.06</v>
       </c>
       <c r="G63" s="1">
-        <v>270.58</v>
+        <v>269.27999999999997</v>
       </c>
       <c r="H63" s="1">
-        <v>262.18</v>
+        <v>262.08</v>
       </c>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
@@ -3142,28 +3150,28 @@
     </row>
     <row r="64" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="2">
-        <v>43479</v>
+        <v>43487</v>
       </c>
       <c r="B64" s="2">
-        <v>43483</v>
+        <v>43490</v>
       </c>
       <c r="C64" s="1">
-        <v>256.86</v>
+        <v>264.82</v>
       </c>
       <c r="D64" s="1">
-        <v>266.98</v>
+        <v>266.7</v>
       </c>
       <c r="E64" s="1">
-        <v>256.41000000000003</v>
+        <v>260.66000000000003</v>
       </c>
       <c r="F64" s="1">
-        <v>266.45999999999998</v>
+        <v>265.77999999999997</v>
       </c>
       <c r="G64" s="1">
-        <v>263.19</v>
+        <v>270.58</v>
       </c>
       <c r="H64" s="1">
-        <v>254.6</v>
+        <v>262.18</v>
       </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
@@ -3187,28 +3195,28 @@
     </row>
     <row r="65" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="2">
-        <v>43472</v>
+        <v>43479</v>
       </c>
       <c r="B65" s="2">
-        <v>43476</v>
+        <v>43483</v>
       </c>
       <c r="C65" s="1">
-        <v>252.69</v>
+        <v>256.86</v>
       </c>
       <c r="D65" s="1">
-        <v>259.16000000000003</v>
+        <v>266.98</v>
       </c>
       <c r="E65" s="1">
-        <v>251.69</v>
+        <v>256.41000000000003</v>
       </c>
       <c r="F65" s="1">
-        <v>258.98</v>
+        <v>266.45999999999998</v>
       </c>
       <c r="G65" s="1">
-        <v>256.42</v>
+        <v>263.19</v>
       </c>
       <c r="H65" s="1">
-        <v>248.22</v>
+        <v>254.6</v>
       </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
@@ -3232,28 +3240,28 @@
     </row>
     <row r="66" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="2">
-        <v>43465</v>
+        <v>43472</v>
       </c>
       <c r="B66" s="2">
-        <v>43469</v>
+        <v>43476</v>
       </c>
       <c r="C66" s="1">
-        <v>249.56</v>
+        <v>252.69</v>
       </c>
       <c r="D66" s="1">
-        <v>253.11</v>
+        <v>259.16000000000003</v>
       </c>
       <c r="E66" s="1">
-        <v>243.67</v>
+        <v>251.69</v>
       </c>
       <c r="F66" s="1">
-        <v>252.39</v>
+        <v>258.98</v>
       </c>
       <c r="G66" s="1">
-        <v>253.59</v>
+        <v>256.42</v>
       </c>
       <c r="H66" s="1">
-        <v>241.95</v>
+        <v>248.22</v>
       </c>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
@@ -3277,28 +3285,28 @@
     </row>
     <row r="67" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="2">
-        <v>43458</v>
+        <v>43465</v>
       </c>
       <c r="B67" s="2">
-        <v>43462</v>
+        <v>43469</v>
       </c>
       <c r="C67" s="1">
-        <v>239.04</v>
+        <v>249.56</v>
       </c>
       <c r="D67" s="1">
-        <v>251.4</v>
+        <v>253.11</v>
       </c>
       <c r="E67" s="1">
-        <v>233.76</v>
+        <v>243.67</v>
       </c>
       <c r="F67" s="1">
-        <v>247.75</v>
+        <v>252.39</v>
       </c>
       <c r="G67" s="1">
-        <v>247.01</v>
+        <v>253.59</v>
       </c>
       <c r="H67" s="1">
-        <v>234.37</v>
+        <v>241.95</v>
       </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
@@ -3322,28 +3330,28 @@
     </row>
     <row r="68" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="2">
-        <v>43451</v>
+        <v>43458</v>
       </c>
       <c r="B68" s="2">
-        <v>43455</v>
+        <v>43462</v>
       </c>
       <c r="C68" s="1">
-        <v>259.39999999999998</v>
+        <v>239.04</v>
       </c>
       <c r="D68" s="1">
-        <v>260.64999999999998</v>
+        <v>251.4</v>
       </c>
       <c r="E68" s="1">
-        <v>239.98</v>
+        <v>233.76</v>
       </c>
       <c r="F68" s="1">
-        <v>240.7</v>
+        <v>247.75</v>
       </c>
       <c r="G68" s="1">
-        <v>266.63</v>
+        <v>247.01</v>
       </c>
       <c r="H68" s="1">
-        <v>254.29</v>
+        <v>234.37</v>
       </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
@@ -3365,6 +3373,51 @@
       <c r="Z68" s="1"/>
       <c r="AA68" s="1"/>
     </row>
+    <row r="69" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="2">
+        <v>43451</v>
+      </c>
+      <c r="B69" s="2">
+        <v>43455</v>
+      </c>
+      <c r="C69" s="1">
+        <v>259.39999999999998</v>
+      </c>
+      <c r="D69" s="1">
+        <v>260.64999999999998</v>
+      </c>
+      <c r="E69" s="1">
+        <v>239.98</v>
+      </c>
+      <c r="F69" s="1">
+        <v>240.7</v>
+      </c>
+      <c r="G69" s="1">
+        <v>266.63</v>
+      </c>
+      <c r="H69" s="1">
+        <v>254.29</v>
+      </c>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+      <c r="Y69" s="1"/>
+      <c r="Z69" s="1"/>
+      <c r="AA69" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add environment file and new data
</commit_message>
<xml_diff>
--- a/ExpectedMove/expected_moves.xlsx
+++ b/ExpectedMove/expected_moves.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dallincoons/Projects/expected_move/ExpectedMove/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83442EC2-C3D2-DD47-8FFD-88CD09F3CA16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1850DBAA-68A0-8941-AD09-2E21DE5BEFEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42500" yWindow="920" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -305,7 +305,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA69"/>
+  <dimension ref="A1:AA70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -360,28 +360,28 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
-        <v>43920</v>
+        <v>43927</v>
       </c>
       <c r="B2" s="2">
-        <v>43924</v>
+        <v>43930</v>
       </c>
       <c r="C2" s="1">
-        <v>255.7</v>
+        <v>257.83999999999997</v>
       </c>
       <c r="D2" s="1">
-        <v>263.33</v>
+        <v>281.2</v>
       </c>
       <c r="E2" s="1">
-        <v>247.6</v>
+        <v>248.17</v>
       </c>
       <c r="F2" s="1">
-        <v>248.89</v>
+        <v>278.2</v>
       </c>
       <c r="G2" s="1">
-        <v>274.065</v>
+        <v>259.94099999999997</v>
       </c>
       <c r="H2" s="1">
-        <v>232.77500000000001</v>
+        <v>236.43899999999999</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -405,28 +405,28 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
-        <v>43913</v>
+        <v>43920</v>
       </c>
       <c r="B3" s="2">
-        <v>43917</v>
+        <v>43924</v>
       </c>
       <c r="C3" s="1">
-        <v>228.19</v>
+        <v>255.7</v>
       </c>
       <c r="D3" s="1">
-        <v>262.8</v>
+        <v>263.33</v>
       </c>
       <c r="E3" s="1">
-        <v>218.26</v>
+        <v>247.6</v>
       </c>
       <c r="F3" s="1">
-        <v>253.42</v>
+        <v>248.89</v>
       </c>
       <c r="G3" s="1">
-        <v>251.554</v>
+        <v>274.065</v>
       </c>
       <c r="H3" s="1">
-        <v>206.04599999999999</v>
+        <v>232.77500000000001</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -450,28 +450,28 @@
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
-        <v>43906</v>
+        <v>43913</v>
       </c>
       <c r="B4" s="2">
-        <v>43910</v>
+        <v>43917</v>
       </c>
       <c r="C4" s="1">
-        <v>241.18</v>
+        <v>228.19</v>
       </c>
       <c r="D4" s="1">
-        <v>256.89999999999998</v>
+        <v>262.8</v>
       </c>
       <c r="E4" s="1">
-        <v>228.02</v>
+        <v>218.26</v>
       </c>
       <c r="F4" s="1">
-        <v>228.8</v>
+        <v>253.42</v>
       </c>
       <c r="G4" s="1">
-        <v>292.32</v>
+        <v>251.554</v>
       </c>
       <c r="H4" s="1">
-        <v>246.32</v>
+        <v>206.04599999999999</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -495,28 +495,28 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
-        <v>43899</v>
+        <v>43906</v>
       </c>
       <c r="B5" s="2">
-        <v>43903</v>
+        <v>43910</v>
       </c>
       <c r="C5" s="1">
-        <v>275.3</v>
+        <v>241.18</v>
       </c>
       <c r="D5" s="1">
-        <v>288.52</v>
+        <v>256.89999999999998</v>
       </c>
       <c r="E5" s="1">
-        <v>247.68</v>
+        <v>228.02</v>
       </c>
       <c r="F5" s="1">
-        <v>248.11</v>
+        <v>228.8</v>
       </c>
       <c r="G5" s="1">
-        <v>313.53199999999998</v>
+        <v>292.32</v>
       </c>
       <c r="H5" s="1">
-        <v>281.38799999999998</v>
+        <v>246.32</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -540,28 +540,28 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
-        <v>43892</v>
+        <v>43899</v>
       </c>
       <c r="B6" s="2">
-        <v>43896</v>
+        <v>43903</v>
       </c>
       <c r="C6" s="1">
-        <v>298.20999999999998</v>
+        <v>275.3</v>
       </c>
       <c r="D6" s="1">
-        <v>313.83999999999997</v>
+        <v>288.52</v>
       </c>
       <c r="E6" s="1">
-        <v>290.23</v>
+        <v>247.68</v>
       </c>
       <c r="F6" s="1">
-        <v>297.45999999999998</v>
+        <v>248.11</v>
       </c>
       <c r="G6" s="1">
-        <v>314.45999999999998</v>
+        <v>313.53199999999998</v>
       </c>
       <c r="H6" s="1">
-        <v>278.06</v>
+        <v>281.38799999999998</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -585,28 +585,28 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
-        <v>43885</v>
+        <v>43892</v>
       </c>
       <c r="B7" s="2">
-        <v>43889</v>
+        <v>43896</v>
       </c>
       <c r="C7" s="1">
-        <v>323.14</v>
+        <v>298.20999999999998</v>
       </c>
       <c r="D7" s="1">
-        <v>337.06</v>
+        <v>313.83999999999997</v>
       </c>
       <c r="E7" s="1">
-        <v>285.54000000000002</v>
+        <v>290.23</v>
       </c>
       <c r="F7" s="1">
-        <v>296.26</v>
+        <v>297.45999999999998</v>
       </c>
       <c r="G7" s="1">
-        <v>338.75</v>
+        <v>314.45999999999998</v>
       </c>
       <c r="H7" s="1">
-        <v>328.24</v>
+        <v>278.06</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -630,28 +630,28 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
-        <v>43879</v>
+        <v>43885</v>
       </c>
       <c r="B8" s="2">
-        <v>43882</v>
+        <v>43889</v>
       </c>
       <c r="C8" s="1">
-        <v>336.51</v>
+        <v>323.14</v>
       </c>
       <c r="D8" s="1">
-        <v>339.08</v>
+        <v>337.06</v>
       </c>
       <c r="E8" s="1">
-        <v>332.58</v>
+        <v>285.54000000000002</v>
       </c>
       <c r="F8" s="1">
-        <v>333.48</v>
+        <v>296.26</v>
       </c>
       <c r="G8" s="1">
-        <v>341.637</v>
+        <v>338.75</v>
       </c>
       <c r="H8" s="1">
-        <v>333.56299999999999</v>
+        <v>328.24</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -675,28 +675,28 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
-        <v>43871</v>
+        <v>43879</v>
       </c>
       <c r="B9" s="2">
-        <v>43875</v>
+        <v>43882</v>
       </c>
       <c r="C9" s="1">
-        <v>331.23</v>
+        <v>336.51</v>
       </c>
       <c r="D9" s="1">
-        <v>338.12</v>
+        <v>339.08</v>
       </c>
       <c r="E9" s="1">
-        <v>331.19</v>
+        <v>332.58</v>
       </c>
       <c r="F9" s="1">
-        <v>337.6</v>
+        <v>333.48</v>
       </c>
       <c r="G9" s="1">
-        <v>337.32600000000002</v>
+        <v>341.637</v>
       </c>
       <c r="H9" s="1">
-        <v>327.07799999999997</v>
+        <v>333.56299999999999</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -720,28 +720,28 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
-        <v>43864</v>
+        <v>43871</v>
       </c>
       <c r="B10" s="2">
-        <v>43868</v>
+        <v>43875</v>
       </c>
       <c r="C10" s="1">
-        <v>323.35000000000002</v>
+        <v>331.23</v>
       </c>
       <c r="D10" s="1">
-        <v>334.49</v>
+        <v>338.12</v>
       </c>
       <c r="E10" s="1">
-        <v>323.22000000000003</v>
+        <v>331.19</v>
       </c>
       <c r="F10" s="1">
-        <v>332.2</v>
+        <v>337.6</v>
       </c>
       <c r="G10" s="1">
-        <v>327.82</v>
+        <v>337.32600000000002</v>
       </c>
       <c r="H10" s="1">
-        <v>315.64</v>
+        <v>327.07799999999997</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -765,28 +765,28 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
-        <v>43857</v>
+        <v>43864</v>
       </c>
       <c r="B11" s="2">
-        <v>43861</v>
+        <v>43868</v>
       </c>
       <c r="C11" s="1">
-        <v>323.02999999999997</v>
+        <v>323.35000000000002</v>
       </c>
       <c r="D11" s="1">
-        <v>328.63</v>
+        <v>334.49</v>
       </c>
       <c r="E11" s="1">
-        <v>320.73</v>
+        <v>323.22000000000003</v>
       </c>
       <c r="F11" s="1">
-        <v>321.73</v>
+        <v>332.2</v>
       </c>
       <c r="G11" s="1">
-        <v>334.03699999999998</v>
+        <v>327.82</v>
       </c>
       <c r="H11" s="1">
-        <v>323.50400000000002</v>
+        <v>315.64</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -810,28 +810,28 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
-        <v>43851</v>
+        <v>43857</v>
       </c>
       <c r="B12" s="2">
-        <v>43854</v>
+        <v>43861</v>
       </c>
       <c r="C12" s="1">
-        <v>332.44</v>
+        <v>323.02999999999997</v>
       </c>
       <c r="D12" s="1">
-        <v>332.53</v>
+        <v>328.63</v>
       </c>
       <c r="E12" s="1">
-        <v>327.36</v>
+        <v>320.73</v>
       </c>
       <c r="F12" s="1">
-        <v>328.77</v>
+        <v>321.73</v>
       </c>
       <c r="G12" s="1">
-        <v>334.07</v>
+        <v>334.03699999999998</v>
       </c>
       <c r="H12" s="1">
-        <v>329.83</v>
+        <v>323.50400000000002</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -855,28 +855,28 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
-        <v>43843</v>
+        <v>43851</v>
       </c>
       <c r="B13" s="2">
-        <v>43847</v>
+        <v>43854</v>
       </c>
       <c r="C13" s="1">
-        <v>326.39</v>
+        <v>332.44</v>
       </c>
       <c r="D13" s="1">
-        <v>332.18</v>
+        <v>332.53</v>
       </c>
       <c r="E13" s="1">
-        <v>325.92</v>
+        <v>327.36</v>
       </c>
       <c r="F13" s="1">
-        <v>331.95</v>
+        <v>328.77</v>
       </c>
       <c r="G13" s="1">
-        <v>329.14</v>
+        <v>334.07</v>
       </c>
       <c r="H13" s="1">
-        <v>322.27999999999997</v>
+        <v>329.83</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -900,28 +900,28 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
-        <v>43836</v>
+        <v>43843</v>
       </c>
       <c r="B14" s="2">
-        <v>43840</v>
+        <v>43847</v>
       </c>
       <c r="C14" s="1">
-        <v>320.49</v>
+        <v>326.39</v>
       </c>
       <c r="D14" s="1">
-        <v>327.45999999999998</v>
+        <v>332.18</v>
       </c>
       <c r="E14" s="1">
-        <v>325.70999999999998</v>
+        <v>325.92</v>
       </c>
       <c r="F14" s="1">
-        <v>325.70999999999998</v>
+        <v>331.95</v>
       </c>
       <c r="G14" s="1">
-        <v>325.54000000000002</v>
+        <v>329.14</v>
       </c>
       <c r="H14" s="1">
-        <v>319.27999999999997</v>
+        <v>322.27999999999997</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -945,28 +945,28 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
-        <v>43829</v>
+        <v>43836</v>
       </c>
       <c r="B15" s="2">
-        <v>43833</v>
+        <v>43840</v>
       </c>
       <c r="C15" s="1">
-        <v>322.95</v>
+        <v>320.49</v>
       </c>
       <c r="D15" s="1">
-        <v>324.89</v>
+        <v>327.45999999999998</v>
       </c>
       <c r="E15" s="1">
-        <v>320.14999999999998</v>
+        <v>325.70999999999998</v>
       </c>
       <c r="F15" s="1">
-        <v>322.41000000000003</v>
+        <v>325.70999999999998</v>
       </c>
       <c r="G15" s="1">
-        <v>326.23</v>
+        <v>325.54000000000002</v>
       </c>
       <c r="H15" s="1">
-        <v>319.5</v>
+        <v>319.27999999999997</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -990,28 +990,28 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
-        <v>43822</v>
+        <v>43829</v>
       </c>
       <c r="B16" s="2">
-        <v>43826</v>
+        <v>43833</v>
       </c>
       <c r="C16" s="1">
-        <v>321.58999999999997</v>
+        <v>322.95</v>
       </c>
       <c r="D16" s="1">
-        <v>323.8</v>
+        <v>324.89</v>
       </c>
       <c r="E16" s="1">
-        <v>320.89999999999998</v>
+        <v>320.14999999999998</v>
       </c>
       <c r="F16" s="1">
-        <v>322.86</v>
+        <v>322.41000000000003</v>
       </c>
       <c r="G16" s="1">
-        <v>324.20999999999998</v>
+        <v>326.23</v>
       </c>
       <c r="H16" s="1">
-        <v>317.23</v>
+        <v>319.5</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1035,28 +1035,28 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
-        <v>43815</v>
+        <v>43822</v>
       </c>
       <c r="B17" s="2">
-        <v>43819</v>
+        <v>43826</v>
       </c>
       <c r="C17" s="1">
-        <v>319.22000000000003</v>
+        <v>321.58999999999997</v>
       </c>
       <c r="D17" s="1">
-        <v>321.97000000000003</v>
+        <v>323.8</v>
       </c>
       <c r="E17" s="1">
-        <v>317.25</v>
+        <v>320.89999999999998</v>
       </c>
       <c r="F17" s="1">
-        <v>320.73</v>
+        <v>322.86</v>
       </c>
       <c r="G17" s="1">
-        <v>320.94</v>
+        <v>324.20999999999998</v>
       </c>
       <c r="H17" s="1">
-        <v>313.70999999999998</v>
+        <v>317.23</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1080,28 +1080,28 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
-        <v>43808</v>
+        <v>43815</v>
       </c>
       <c r="B18" s="2">
-        <v>43812</v>
+        <v>43819</v>
       </c>
       <c r="C18" s="1">
-        <v>314.44</v>
+        <v>319.22000000000003</v>
       </c>
       <c r="D18" s="1">
-        <v>318.67</v>
+        <v>321.97000000000003</v>
       </c>
       <c r="E18" s="1">
-        <v>312.81</v>
+        <v>317.25</v>
       </c>
       <c r="F18" s="1">
-        <v>317.32</v>
+        <v>320.73</v>
       </c>
       <c r="G18" s="1">
-        <v>318.19</v>
+        <v>320.94</v>
       </c>
       <c r="H18" s="1">
-        <v>311.56</v>
+        <v>313.70999999999998</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1125,28 +1125,28 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
-        <v>43801</v>
+        <v>43808</v>
       </c>
       <c r="B19" s="2">
-        <v>43805</v>
+        <v>43812</v>
       </c>
       <c r="C19" s="1">
-        <v>314.58999999999997</v>
+        <v>314.44</v>
       </c>
       <c r="D19" s="1">
-        <v>315.31</v>
+        <v>318.67</v>
       </c>
       <c r="E19" s="1">
-        <v>307.13</v>
+        <v>312.81</v>
       </c>
       <c r="F19" s="1">
-        <v>314.87</v>
+        <v>317.32</v>
       </c>
       <c r="G19" s="1">
-        <v>317.69</v>
+        <v>318.19</v>
       </c>
       <c r="H19" s="1">
-        <v>310.92</v>
+        <v>311.56</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1170,28 +1170,28 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
-        <v>43794</v>
+        <v>43801</v>
       </c>
       <c r="B20" s="2">
-        <v>43798</v>
+        <v>43805</v>
       </c>
       <c r="C20" s="1">
-        <v>311.98</v>
+        <v>314.58999999999997</v>
       </c>
       <c r="D20" s="1">
-        <v>315.48</v>
+        <v>315.31</v>
       </c>
       <c r="E20" s="1">
-        <v>311.98</v>
+        <v>307.13</v>
       </c>
       <c r="F20" s="1">
-        <v>314.31</v>
+        <v>314.87</v>
       </c>
       <c r="G20" s="1">
-        <v>314.56</v>
+        <v>317.69</v>
       </c>
       <c r="H20" s="1">
-        <v>307.39</v>
+        <v>310.92</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1215,28 +1215,28 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
-        <v>43787</v>
+        <v>43794</v>
       </c>
       <c r="B21" s="2">
-        <v>43791</v>
+        <v>43798</v>
       </c>
       <c r="C21" s="1">
-        <v>311.52999999999997</v>
+        <v>311.98</v>
       </c>
       <c r="D21" s="1">
-        <v>312.69</v>
+        <v>315.48</v>
       </c>
       <c r="E21" s="1">
-        <v>309.06</v>
+        <v>311.98</v>
       </c>
       <c r="F21" s="1">
-        <v>310.95999999999998</v>
+        <v>314.31</v>
       </c>
       <c r="G21" s="1">
-        <v>315.3</v>
+        <v>314.56</v>
       </c>
       <c r="H21" s="1">
-        <v>308.25</v>
+        <v>307.39</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1260,28 +1260,28 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
-        <v>43780</v>
+        <v>43787</v>
       </c>
       <c r="B22" s="2">
-        <v>43784</v>
+        <v>43791</v>
       </c>
       <c r="C22" s="1">
-        <v>307.42</v>
+        <v>311.52999999999997</v>
       </c>
       <c r="D22" s="1">
-        <v>311.83999999999997</v>
+        <v>312.69</v>
       </c>
       <c r="E22" s="1">
-        <v>307.27</v>
+        <v>309.06</v>
       </c>
       <c r="F22" s="1">
-        <v>311.79000000000002</v>
+        <v>310.95999999999998</v>
       </c>
       <c r="G22" s="1">
-        <v>312.52</v>
+        <v>315.3</v>
       </c>
       <c r="H22" s="1">
-        <v>305.36</v>
+        <v>308.25</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1305,28 +1305,28 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
-        <v>43773</v>
+        <v>43780</v>
       </c>
       <c r="B23" s="2">
-        <v>43777</v>
+        <v>43784</v>
       </c>
       <c r="C23" s="1">
-        <v>307.85000000000002</v>
+        <v>307.42</v>
       </c>
       <c r="D23" s="1">
-        <v>309.64999999999998</v>
+        <v>311.83999999999997</v>
       </c>
       <c r="E23" s="1">
-        <v>306.06</v>
+        <v>307.27</v>
       </c>
       <c r="F23" s="1">
-        <v>308.94</v>
+        <v>311.79000000000002</v>
       </c>
       <c r="G23" s="1">
-        <v>309.85000000000002</v>
+        <v>312.52</v>
       </c>
       <c r="H23" s="1">
-        <v>302.44</v>
+        <v>305.36</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1350,28 +1350,28 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
-        <v>43766</v>
+        <v>43773</v>
       </c>
       <c r="B24" s="2">
-        <v>43770</v>
+        <v>43777</v>
       </c>
       <c r="C24" s="1">
-        <v>302.94</v>
+        <v>307.85000000000002</v>
       </c>
       <c r="D24" s="1">
-        <v>306.19</v>
+        <v>309.64999999999998</v>
       </c>
       <c r="E24" s="1">
-        <v>301.73</v>
+        <v>306.06</v>
       </c>
       <c r="F24" s="1">
-        <v>306.14</v>
+        <v>308.94</v>
       </c>
       <c r="G24" s="1">
-        <v>305.2</v>
+        <v>309.85000000000002</v>
       </c>
       <c r="H24" s="1">
-        <v>298.01</v>
+        <v>302.44</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1395,28 +1395,28 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
-        <v>43759</v>
+        <v>43766</v>
       </c>
       <c r="B25" s="2">
-        <v>43763</v>
+        <v>43770</v>
       </c>
       <c r="C25" s="1">
-        <v>299.42</v>
+        <v>302.94</v>
       </c>
       <c r="D25" s="1">
-        <v>302.2</v>
+        <v>306.19</v>
       </c>
       <c r="E25" s="1">
-        <v>298.5</v>
+        <v>301.73</v>
       </c>
       <c r="F25" s="1">
-        <v>301.60000000000002</v>
+        <v>306.14</v>
       </c>
       <c r="G25" s="1">
-        <v>301.77999999999997</v>
+        <v>305.2</v>
       </c>
       <c r="H25" s="1">
-        <v>294.14999999999998</v>
+        <v>298.01</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1440,28 +1440,28 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
-        <v>43752</v>
+        <v>43759</v>
       </c>
       <c r="B26" s="2">
-        <v>43756</v>
+        <v>43763</v>
       </c>
       <c r="C26" s="1">
-        <v>295.93</v>
+        <v>299.42</v>
       </c>
       <c r="D26" s="1">
-        <v>300.24</v>
+        <v>302.2</v>
       </c>
       <c r="E26" s="1">
-        <v>295.57</v>
+        <v>298.5</v>
       </c>
       <c r="F26" s="1">
-        <v>297.97000000000003</v>
+        <v>301.60000000000002</v>
       </c>
       <c r="G26" s="1">
-        <v>300.29000000000002</v>
+        <v>301.77999999999997</v>
       </c>
       <c r="H26" s="1">
-        <v>292.26</v>
+        <v>294.14999999999998</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1485,28 +1485,28 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
-        <v>43745</v>
+        <v>43752</v>
       </c>
       <c r="B27" s="2">
-        <v>43749</v>
+        <v>43756</v>
       </c>
       <c r="C27" s="1">
-        <v>293.47000000000003</v>
+        <v>295.93</v>
       </c>
       <c r="D27" s="1">
-        <v>298.74</v>
+        <v>300.24</v>
       </c>
       <c r="E27" s="1">
-        <v>288.49</v>
+        <v>295.57</v>
       </c>
       <c r="F27" s="1">
-        <v>296.27999999999997</v>
+        <v>297.97000000000003</v>
       </c>
       <c r="G27" s="1">
-        <v>298.93</v>
+        <v>300.29000000000002</v>
       </c>
       <c r="H27" s="1">
-        <v>289.74</v>
+        <v>292.26</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1530,28 +1530,28 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
-        <v>43738</v>
+        <v>43745</v>
       </c>
       <c r="B28" s="2">
-        <v>43742</v>
+        <v>43749</v>
       </c>
       <c r="C28" s="1">
-        <v>295.97000000000003</v>
+        <v>293.47000000000003</v>
       </c>
       <c r="D28" s="1">
-        <v>298.45999999999998</v>
+        <v>298.74</v>
       </c>
       <c r="E28" s="1">
-        <v>284.82</v>
+        <v>288.49</v>
       </c>
       <c r="F28" s="1">
-        <v>294.35000000000002</v>
+        <v>296.27999999999997</v>
       </c>
       <c r="G28" s="1">
-        <v>300.01</v>
+        <v>298.93</v>
       </c>
       <c r="H28" s="1">
-        <v>290.77999999999997</v>
+        <v>289.74</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1575,28 +1575,28 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
-        <v>43731</v>
+        <v>43738</v>
       </c>
       <c r="B29" s="2">
-        <v>43735</v>
+        <v>43742</v>
       </c>
       <c r="C29" s="1">
-        <v>297.55</v>
+        <v>295.97000000000003</v>
       </c>
       <c r="D29" s="1">
-        <v>299.83999999999997</v>
+        <v>298.45999999999998</v>
       </c>
       <c r="E29" s="1">
-        <v>293.69</v>
+        <v>284.82</v>
       </c>
       <c r="F29" s="1">
-        <v>295.39999999999998</v>
+        <v>294.35000000000002</v>
       </c>
       <c r="G29" s="1">
-        <v>302.43</v>
+        <v>300.01</v>
       </c>
       <c r="H29" s="1">
-        <v>294.13</v>
+        <v>290.77999999999997</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1620,28 +1620,28 @@
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
-        <v>43724</v>
+        <v>43731</v>
       </c>
       <c r="B30" s="2">
-        <v>43728</v>
+        <v>43735</v>
       </c>
       <c r="C30" s="1">
+        <v>297.55</v>
+      </c>
+      <c r="D30" s="1">
         <v>299.83999999999997</v>
       </c>
-      <c r="D30" s="1">
-        <v>302.63</v>
-      </c>
       <c r="E30" s="1">
-        <v>297.41000000000003</v>
+        <v>293.69</v>
       </c>
       <c r="F30" s="1">
-        <v>298.27999999999997</v>
+        <v>295.39999999999998</v>
       </c>
       <c r="G30" s="1">
-        <v>304.77999999999997</v>
+        <v>302.43</v>
       </c>
       <c r="H30" s="1">
-        <v>297.39999999999998</v>
+        <v>294.13</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -1665,28 +1665,28 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
-        <v>43717</v>
+        <v>43724</v>
       </c>
       <c r="B31" s="2">
-        <v>43721</v>
+        <v>43728</v>
       </c>
       <c r="C31" s="1">
-        <v>299.14</v>
+        <v>299.83999999999997</v>
       </c>
       <c r="D31" s="1">
-        <v>302.45999999999998</v>
+        <v>302.63</v>
       </c>
       <c r="E31" s="1">
-        <v>295.97000000000003</v>
+        <v>297.41000000000003</v>
       </c>
       <c r="F31" s="1">
-        <v>301.08999999999997</v>
+        <v>298.27999999999997</v>
       </c>
       <c r="G31" s="1">
-        <v>302.2</v>
+        <v>304.77999999999997</v>
       </c>
       <c r="H31" s="1">
-        <v>293.89999999999998</v>
+        <v>297.39999999999998</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1710,28 +1710,28 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
-        <v>43711</v>
+        <v>43717</v>
       </c>
       <c r="B32" s="2">
-        <v>43714</v>
+        <v>43721</v>
       </c>
       <c r="C32" s="1">
-        <v>290.57</v>
+        <v>299.14</v>
       </c>
       <c r="D32" s="1">
-        <v>298.83</v>
+        <v>302.45999999999998</v>
       </c>
       <c r="E32" s="1">
-        <v>289.27</v>
+        <v>295.97000000000003</v>
       </c>
       <c r="F32" s="1">
-        <v>298.05</v>
+        <v>301.08999999999997</v>
       </c>
       <c r="G32" s="1">
-        <v>297.49</v>
+        <v>302.2</v>
       </c>
       <c r="H32" s="1">
-        <v>287.39</v>
+        <v>293.89999999999998</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1755,28 +1755,28 @@
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
-        <v>43703</v>
+        <v>43711</v>
       </c>
       <c r="B33" s="2">
-        <v>43707</v>
+        <v>43714</v>
       </c>
       <c r="C33" s="1">
-        <v>287.27</v>
+        <v>290.57</v>
       </c>
       <c r="D33" s="1">
-        <v>294.24</v>
+        <v>298.83</v>
       </c>
       <c r="E33" s="1">
-        <v>285.25</v>
+        <v>289.27</v>
       </c>
       <c r="F33" s="1">
-        <v>292.45</v>
+        <v>298.05</v>
       </c>
       <c r="G33" s="1">
-        <v>290.10000000000002</v>
+        <v>297.49</v>
       </c>
       <c r="H33" s="1">
-        <v>279.60000000000002</v>
+        <v>287.39</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1800,28 +1800,28 @@
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
-        <v>43696</v>
+        <v>43703</v>
       </c>
       <c r="B34" s="2">
-        <v>43700</v>
+        <v>43707</v>
       </c>
       <c r="C34" s="1">
-        <v>292.19</v>
+        <v>287.27</v>
       </c>
       <c r="D34" s="1">
-        <v>293.93</v>
+        <v>294.24</v>
       </c>
       <c r="E34" s="1">
-        <v>283.47000000000003</v>
+        <v>285.25</v>
       </c>
       <c r="F34" s="1">
-        <v>284.85000000000002</v>
+        <v>292.45</v>
       </c>
       <c r="G34" s="1">
-        <v>293.75</v>
+        <v>290.10000000000002</v>
       </c>
       <c r="H34" s="1">
-        <v>283.94</v>
+        <v>279.60000000000002</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1845,28 +1845,28 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
-        <v>43689</v>
+        <v>43696</v>
       </c>
       <c r="B35" s="2">
-        <v>43693</v>
+        <v>43700</v>
       </c>
       <c r="C35" s="1">
-        <v>289.95999999999998</v>
+        <v>292.19</v>
       </c>
       <c r="D35" s="1">
-        <v>294.14999999999998</v>
+        <v>293.93</v>
       </c>
       <c r="E35" s="1">
-        <v>282.39</v>
+        <v>283.47000000000003</v>
       </c>
       <c r="F35" s="1">
-        <v>288.85000000000002</v>
+        <v>284.85000000000002</v>
       </c>
       <c r="G35" s="1">
-        <v>296.31</v>
+        <v>293.75</v>
       </c>
       <c r="H35" s="1">
-        <v>286.95</v>
+        <v>283.94</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -1890,28 +1890,28 @@
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
-        <v>43682</v>
+        <v>43689</v>
       </c>
       <c r="B36" s="2">
-        <v>43686</v>
+        <v>43693</v>
       </c>
       <c r="C36" s="1">
-        <v>288.08999999999997</v>
+        <v>289.95999999999998</v>
       </c>
       <c r="D36" s="1">
-        <v>293.62</v>
+        <v>294.14999999999998</v>
       </c>
       <c r="E36" s="1">
-        <v>281.72000000000003</v>
+        <v>282.39</v>
       </c>
       <c r="F36" s="1">
-        <v>291.62</v>
+        <v>288.85000000000002</v>
       </c>
       <c r="G36" s="1">
-        <v>296.85000000000002</v>
+        <v>296.31</v>
       </c>
       <c r="H36" s="1">
-        <v>288.33</v>
+        <v>286.95</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -1935,28 +1935,28 @@
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
-        <v>43675</v>
+        <v>43682</v>
       </c>
       <c r="B37" s="2">
-        <v>43679</v>
+        <v>43686</v>
       </c>
       <c r="C37" s="1">
-        <v>301.88</v>
+        <v>288.08999999999997</v>
       </c>
       <c r="D37" s="1">
-        <v>301.93</v>
+        <v>293.62</v>
       </c>
       <c r="E37" s="1">
-        <v>290.89999999999998</v>
+        <v>281.72000000000003</v>
       </c>
       <c r="F37" s="1">
-        <v>292.62</v>
+        <v>291.62</v>
       </c>
       <c r="G37" s="1">
-        <v>305.18</v>
+        <v>296.85000000000002</v>
       </c>
       <c r="H37" s="1">
-        <v>298.86</v>
+        <v>288.33</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -1980,28 +1980,28 @@
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
-        <v>43668</v>
+        <v>43675</v>
       </c>
       <c r="B38" s="2">
-        <v>43672</v>
+        <v>43679</v>
       </c>
       <c r="C38" s="1">
-        <v>297.61</v>
+        <v>301.88</v>
       </c>
       <c r="D38" s="1">
-        <v>302.23</v>
+        <v>301.93</v>
       </c>
       <c r="E38" s="1">
-        <v>297.04000000000002</v>
+        <v>290.89999999999998</v>
       </c>
       <c r="F38" s="1">
-        <v>302.01</v>
+        <v>292.62</v>
       </c>
       <c r="G38" s="1">
-        <v>301.06</v>
+        <v>305.18</v>
       </c>
       <c r="H38" s="1">
-        <v>293.26</v>
+        <v>298.86</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2025,28 +2025,28 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
-        <v>43661</v>
+        <v>43668</v>
       </c>
       <c r="B39" s="2">
-        <v>43665</v>
+        <v>43672</v>
       </c>
       <c r="C39" s="1">
-        <v>301.13</v>
+        <v>297.61</v>
       </c>
       <c r="D39" s="1">
-        <v>301.13</v>
+        <v>302.23</v>
       </c>
       <c r="E39" s="1">
-        <v>296.7</v>
+        <v>297.04000000000002</v>
       </c>
       <c r="F39" s="1">
-        <v>297.17</v>
+        <v>302.01</v>
       </c>
       <c r="G39" s="1">
-        <v>303.86</v>
+        <v>301.06</v>
       </c>
       <c r="H39" s="1">
-        <v>297.49</v>
+        <v>293.26</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -2070,28 +2070,28 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
-        <v>43654</v>
+        <v>43661</v>
       </c>
       <c r="B40" s="2">
-        <v>43658</v>
+        <v>43665</v>
       </c>
       <c r="C40" s="1">
-        <v>297.01</v>
+        <v>301.13</v>
       </c>
       <c r="D40" s="1">
-        <v>300.73</v>
+        <v>301.13</v>
       </c>
       <c r="E40" s="1">
-        <v>295.48</v>
+        <v>296.7</v>
       </c>
       <c r="F40" s="1">
-        <v>300.64999999999998</v>
+        <v>297.17</v>
       </c>
       <c r="G40" s="1">
-        <v>301.94</v>
+        <v>303.86</v>
       </c>
       <c r="H40" s="1">
-        <v>295</v>
+        <v>297.49</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -2115,28 +2115,28 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
-        <v>43647</v>
+        <v>43654</v>
       </c>
       <c r="B41" s="2">
-        <v>43651</v>
+        <v>43658</v>
       </c>
       <c r="C41" s="1">
-        <v>296.68</v>
+        <v>297.01</v>
       </c>
       <c r="D41" s="1">
-        <v>298.82</v>
+        <v>300.73</v>
       </c>
       <c r="E41" s="1">
-        <v>294.33</v>
+        <v>295.48</v>
       </c>
       <c r="F41" s="1">
-        <v>298.45999999999998</v>
+        <v>300.64999999999998</v>
       </c>
       <c r="G41" s="1">
-        <v>296.95999999999998</v>
+        <v>301.94</v>
       </c>
       <c r="H41" s="1">
-        <v>289.04000000000002</v>
+        <v>295</v>
       </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -2160,28 +2160,28 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
-        <v>43640</v>
+        <v>43647</v>
       </c>
       <c r="B42" s="2">
-        <v>43644</v>
+        <v>43651</v>
       </c>
       <c r="C42" s="1">
-        <v>294.23</v>
+        <v>296.68</v>
       </c>
       <c r="D42" s="1">
-        <v>294.58</v>
+        <v>298.82</v>
       </c>
       <c r="E42" s="1">
-        <v>290.35000000000002</v>
+        <v>294.33</v>
       </c>
       <c r="F42" s="1">
-        <v>293</v>
+        <v>298.45999999999998</v>
       </c>
       <c r="G42" s="1">
-        <v>298.08999999999997</v>
+        <v>296.95999999999998</v>
       </c>
       <c r="H42" s="1">
-        <v>289.87</v>
+        <v>289.04000000000002</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -2205,28 +2205,28 @@
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
-        <v>43633</v>
+        <v>43640</v>
       </c>
       <c r="B43" s="2">
-        <v>43637</v>
+        <v>43644</v>
       </c>
       <c r="C43" s="1">
-        <v>289.52</v>
+        <v>294.23</v>
       </c>
       <c r="D43" s="1">
-        <v>296.31</v>
+        <v>294.58</v>
       </c>
       <c r="E43" s="1">
-        <v>289.18</v>
+        <v>290.35000000000002</v>
       </c>
       <c r="F43" s="1">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G43" s="1">
-        <v>293.19</v>
+        <v>298.08999999999997</v>
       </c>
       <c r="H43" s="1">
-        <v>285.33999999999997</v>
+        <v>289.87</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -2250,28 +2250,28 @@
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
-        <v>43626</v>
+        <v>43633</v>
       </c>
       <c r="B44" s="2">
-        <v>43630</v>
+        <v>43637</v>
       </c>
       <c r="C44" s="1">
-        <v>289.37</v>
+        <v>289.52</v>
       </c>
       <c r="D44" s="1">
-        <v>291.39999999999998</v>
+        <v>296.31</v>
       </c>
       <c r="E44" s="1">
-        <v>287.82</v>
+        <v>289.18</v>
       </c>
       <c r="F44" s="1">
-        <v>289.26</v>
+        <v>294</v>
       </c>
       <c r="G44" s="1">
-        <v>291.85000000000002</v>
+        <v>293.19</v>
       </c>
       <c r="H44" s="1">
-        <v>283.44</v>
+        <v>285.33999999999997</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -2295,28 +2295,28 @@
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
-        <v>43619</v>
+        <v>43626</v>
       </c>
       <c r="B45" s="2">
-        <v>43623</v>
+        <v>43630</v>
       </c>
       <c r="C45" s="1">
-        <v>275.31</v>
+        <v>289.37</v>
       </c>
       <c r="D45" s="1">
-        <v>288.85000000000002</v>
+        <v>291.39999999999998</v>
       </c>
       <c r="E45" s="1">
-        <v>273.08999999999997</v>
+        <v>287.82</v>
       </c>
       <c r="F45" s="1">
-        <v>287.64999999999998</v>
+        <v>289.26</v>
       </c>
       <c r="G45" s="1">
-        <v>279.93</v>
+        <v>291.85000000000002</v>
       </c>
       <c r="H45" s="1">
-        <v>270.63</v>
+        <v>283.44</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -2340,28 +2340,28 @@
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
-        <v>43613</v>
+        <v>43619</v>
       </c>
       <c r="B46" s="2">
-        <v>43616</v>
+        <v>43623</v>
       </c>
       <c r="C46" s="1">
-        <v>283.08999999999997</v>
+        <v>275.31</v>
       </c>
       <c r="D46" s="1">
-        <v>284.14999999999998</v>
+        <v>288.85000000000002</v>
       </c>
       <c r="E46" s="1">
-        <v>275.24</v>
+        <v>273.08999999999997</v>
       </c>
       <c r="F46" s="1">
-        <v>275.27</v>
+        <v>287.64999999999998</v>
       </c>
       <c r="G46" s="1">
-        <v>286.89999999999998</v>
+        <v>279.93</v>
       </c>
       <c r="H46" s="1">
-        <v>278.63</v>
+        <v>270.63</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -2385,28 +2385,28 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
-        <v>43605</v>
+        <v>43613</v>
       </c>
       <c r="B47" s="2">
-        <v>43609</v>
+        <v>43616</v>
       </c>
       <c r="C47" s="1">
-        <v>284.06</v>
+        <v>283.08999999999997</v>
       </c>
       <c r="D47" s="1">
-        <v>286.93</v>
+        <v>284.14999999999998</v>
       </c>
       <c r="E47" s="1">
-        <v>280.57</v>
+        <v>275.24</v>
       </c>
       <c r="F47" s="1">
-        <v>282.77999999999997</v>
+        <v>275.27</v>
       </c>
       <c r="G47" s="1">
-        <v>290</v>
+        <v>286.89999999999998</v>
       </c>
       <c r="H47" s="1">
-        <v>281.63</v>
+        <v>278.63</v>
       </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
@@ -2430,28 +2430,28 @@
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
-        <v>43598</v>
+        <v>43605</v>
       </c>
       <c r="B48" s="2">
-        <v>43602</v>
+        <v>43609</v>
       </c>
       <c r="C48" s="1">
-        <v>282.42</v>
+        <v>284.06</v>
       </c>
       <c r="D48" s="1">
-        <v>289.20999999999998</v>
+        <v>286.93</v>
       </c>
       <c r="E48" s="1">
-        <v>279.93</v>
+        <v>280.57</v>
       </c>
       <c r="F48" s="1">
-        <v>285.83999999999997</v>
+        <v>282.77999999999997</v>
       </c>
       <c r="G48" s="1">
-        <v>292.32</v>
+        <v>290</v>
       </c>
       <c r="H48" s="1">
-        <v>283.8</v>
+        <v>281.63</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -2475,28 +2475,28 @@
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
-        <v>43591</v>
+        <v>43598</v>
       </c>
       <c r="B49" s="2">
-        <v>43595</v>
+        <v>43602</v>
       </c>
       <c r="C49" s="1">
-        <v>289.25</v>
+        <v>282.42</v>
       </c>
       <c r="D49" s="1">
-        <v>293.31</v>
+        <v>289.20999999999998</v>
       </c>
       <c r="E49" s="1">
-        <v>282.3</v>
+        <v>279.93</v>
       </c>
       <c r="F49" s="1">
-        <v>288.10000000000002</v>
+        <v>285.83999999999997</v>
       </c>
       <c r="G49" s="1">
-        <v>297.17</v>
+        <v>292.32</v>
       </c>
       <c r="H49" s="1">
-        <v>290.87</v>
+        <v>283.8</v>
       </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
@@ -2520,28 +2520,28 @@
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
-        <v>43584</v>
+        <v>43591</v>
       </c>
       <c r="B50" s="2">
-        <v>43588</v>
+        <v>43595</v>
       </c>
       <c r="C50" s="1">
-        <v>293.51</v>
+        <v>289.25</v>
       </c>
       <c r="D50" s="1">
-        <v>294.95</v>
+        <v>293.31</v>
       </c>
       <c r="E50" s="1">
-        <v>289.52</v>
+        <v>282.3</v>
       </c>
       <c r="F50" s="1">
-        <v>294.02999999999997</v>
+        <v>288.10000000000002</v>
       </c>
       <c r="G50" s="1">
-        <v>296.5</v>
+        <v>297.17</v>
       </c>
       <c r="H50" s="1">
-        <v>290.25</v>
+        <v>290.87</v>
       </c>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
@@ -2565,28 +2565,28 @@
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
-        <v>43577</v>
+        <v>43584</v>
       </c>
       <c r="B51" s="2">
-        <v>43581</v>
+        <v>43588</v>
       </c>
       <c r="C51" s="1">
-        <v>289.17</v>
+        <v>293.51</v>
       </c>
       <c r="D51" s="1">
-        <v>293.49</v>
+        <v>294.95</v>
       </c>
       <c r="E51" s="1">
-        <v>289.07</v>
+        <v>289.52</v>
       </c>
       <c r="F51" s="1">
-        <v>293.41000000000003</v>
+        <v>294.02999999999997</v>
       </c>
       <c r="G51" s="1">
-        <v>293.19</v>
+        <v>296.5</v>
       </c>
       <c r="H51" s="1">
-        <v>286.85000000000002</v>
+        <v>290.25</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
@@ -2610,28 +2610,28 @@
     </row>
     <row r="52" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2">
-        <v>43570</v>
+        <v>43577</v>
       </c>
       <c r="B52" s="2">
-        <v>43574</v>
+        <v>43581</v>
       </c>
       <c r="C52" s="1">
-        <v>290.24</v>
+        <v>289.17</v>
       </c>
       <c r="D52" s="1">
-        <v>291.43</v>
+        <v>293.49</v>
       </c>
       <c r="E52" s="1">
-        <v>288.66000000000003</v>
+        <v>289.07</v>
       </c>
       <c r="F52" s="1">
-        <v>290.02</v>
+        <v>293.41000000000003</v>
       </c>
       <c r="G52" s="1">
         <v>293.19</v>
       </c>
       <c r="H52" s="1">
-        <v>287.14</v>
+        <v>286.85000000000002</v>
       </c>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
@@ -2655,28 +2655,28 @@
     </row>
     <row r="53" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="2">
-        <v>43563</v>
+        <v>43570</v>
       </c>
       <c r="B53" s="2">
-        <v>43567</v>
+        <v>43574</v>
       </c>
       <c r="C53" s="1">
-        <v>288.10000000000002</v>
+        <v>290.24</v>
       </c>
       <c r="D53" s="1">
-        <v>290.47000000000003</v>
+        <v>291.43</v>
       </c>
       <c r="E53" s="1">
-        <v>286.7</v>
+        <v>288.66000000000003</v>
       </c>
       <c r="F53" s="1">
-        <v>290.16000000000003</v>
+        <v>290.02</v>
       </c>
       <c r="G53" s="1">
-        <v>291.89999999999998</v>
+        <v>293.19</v>
       </c>
       <c r="H53" s="1">
-        <v>285.2</v>
+        <v>287.14</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
@@ -2700,28 +2700,28 @@
     </row>
     <row r="54" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="2">
-        <v>43556</v>
+        <v>43563</v>
       </c>
       <c r="B54" s="2">
-        <v>43560</v>
+        <v>43567</v>
       </c>
       <c r="C54" s="1">
-        <v>284.7</v>
+        <v>288.10000000000002</v>
       </c>
       <c r="D54" s="1">
-        <v>288.63</v>
+        <v>290.47000000000003</v>
       </c>
       <c r="E54" s="1">
-        <v>284.39999999999998</v>
+        <v>286.7</v>
       </c>
       <c r="F54" s="1">
-        <v>288.57</v>
+        <v>290.16000000000003</v>
       </c>
       <c r="G54" s="1">
-        <v>286.06</v>
+        <v>291.89999999999998</v>
       </c>
       <c r="H54" s="1">
-        <v>278.93</v>
+        <v>285.2</v>
       </c>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
@@ -2745,28 +2745,28 @@
     </row>
     <row r="55" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="2">
-        <v>43549</v>
+        <v>43556</v>
       </c>
       <c r="B55" s="2">
-        <v>43553</v>
+        <v>43560</v>
       </c>
       <c r="C55" s="1">
-        <v>278.87</v>
+        <v>284.7</v>
       </c>
       <c r="D55" s="1">
-        <v>282.83999999999997</v>
+        <v>288.63</v>
       </c>
       <c r="E55" s="1">
-        <v>277.64</v>
+        <v>284.39999999999998</v>
       </c>
       <c r="F55" s="1">
-        <v>282.48</v>
+        <v>288.57</v>
       </c>
       <c r="G55" s="1">
-        <v>283.33</v>
+        <v>286.06</v>
       </c>
       <c r="H55" s="1">
-        <v>275.11</v>
+        <v>278.93</v>
       </c>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
@@ -2790,28 +2790,28 @@
     </row>
     <row r="56" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="2">
-        <v>43542</v>
+        <v>43549</v>
       </c>
       <c r="B56" s="2">
-        <v>43546</v>
+        <v>43553</v>
       </c>
       <c r="C56" s="1">
-        <v>281.55</v>
+        <v>278.87</v>
       </c>
       <c r="D56" s="1">
-        <v>285.18</v>
+        <v>282.83999999999997</v>
       </c>
       <c r="E56" s="1">
-        <v>279.18</v>
+        <v>277.64</v>
       </c>
       <c r="F56" s="1">
-        <v>279.25</v>
+        <v>282.48</v>
       </c>
       <c r="G56" s="1">
-        <v>284.55</v>
+        <v>283.33</v>
       </c>
       <c r="H56" s="1">
-        <v>278.14</v>
+        <v>275.11</v>
       </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
@@ -2835,28 +2835,28 @@
     </row>
     <row r="57" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="2">
-        <v>43535</v>
+        <v>43542</v>
       </c>
       <c r="B57" s="2">
-        <v>43539</v>
+        <v>43546</v>
       </c>
       <c r="C57" s="1">
-        <v>275.26</v>
+        <v>281.55</v>
       </c>
       <c r="D57" s="1">
-        <v>282.38</v>
+        <v>285.18</v>
       </c>
       <c r="E57" s="1">
-        <v>275.23</v>
+        <v>279.18</v>
       </c>
       <c r="F57" s="1">
-        <v>281.31</v>
+        <v>279.25</v>
       </c>
       <c r="G57" s="1">
-        <v>278.36</v>
+        <v>284.55</v>
       </c>
       <c r="H57" s="1">
-        <v>270.58</v>
+        <v>278.14</v>
       </c>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
@@ -2880,28 +2880,28 @@
     </row>
     <row r="58" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="2">
-        <v>43528</v>
+        <v>43535</v>
       </c>
       <c r="B58" s="2">
-        <v>43532</v>
+        <v>43539</v>
       </c>
       <c r="C58" s="1">
-        <v>281.60000000000002</v>
+        <v>275.26</v>
       </c>
       <c r="D58" s="1">
-        <v>281.87</v>
+        <v>282.38</v>
       </c>
       <c r="E58" s="1">
-        <v>272.42</v>
+        <v>275.23</v>
       </c>
       <c r="F58" s="1">
-        <v>274.45999999999998</v>
+        <v>281.31</v>
       </c>
       <c r="G58" s="1">
-        <v>283.89999999999998</v>
+        <v>278.36</v>
       </c>
       <c r="H58" s="1">
-        <v>276.92</v>
+        <v>270.58</v>
       </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
@@ -2925,28 +2925,28 @@
     </row>
     <row r="59" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="2">
-        <v>43521</v>
+        <v>43528</v>
       </c>
       <c r="B59" s="2">
-        <v>43525</v>
+        <v>43532</v>
       </c>
       <c r="C59" s="1">
-        <v>280.73</v>
+        <v>281.60000000000002</v>
       </c>
       <c r="D59" s="1">
-        <v>281.31</v>
+        <v>281.87</v>
       </c>
       <c r="E59" s="1">
-        <v>277.48</v>
+        <v>272.42</v>
       </c>
       <c r="F59" s="1">
-        <v>280.42</v>
+        <v>274.45999999999998</v>
       </c>
       <c r="G59" s="1">
-        <v>282.52</v>
+        <v>283.89999999999998</v>
       </c>
       <c r="H59" s="1">
-        <v>275.62</v>
+        <v>276.92</v>
       </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
@@ -2970,28 +2970,28 @@
     </row>
     <row r="60" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="2">
-        <v>43515</v>
+        <v>43521</v>
       </c>
       <c r="B60" s="2">
-        <v>43518</v>
+        <v>43525</v>
       </c>
       <c r="C60" s="1">
-        <v>276.48</v>
+        <v>280.73</v>
       </c>
       <c r="D60" s="1">
-        <v>279.36</v>
+        <v>281.31</v>
       </c>
       <c r="E60" s="1">
-        <v>276.35000000000002</v>
+        <v>277.48</v>
       </c>
       <c r="F60" s="1">
-        <v>279.14</v>
+        <v>280.42</v>
       </c>
       <c r="G60" s="1">
-        <v>281.24</v>
+        <v>282.52</v>
       </c>
       <c r="H60" s="1">
-        <v>273.45999999999998</v>
+        <v>275.62</v>
       </c>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
@@ -3015,28 +3015,28 @@
     </row>
     <row r="61" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="2">
-        <v>43507</v>
+        <v>43515</v>
       </c>
       <c r="B61" s="2">
-        <v>43511</v>
+        <v>43518</v>
       </c>
       <c r="C61" s="1">
-        <v>271.2</v>
+        <v>276.48</v>
       </c>
       <c r="D61" s="1">
-        <v>277.41000000000003</v>
+        <v>279.36</v>
       </c>
       <c r="E61" s="1">
-        <v>270.02999999999997</v>
+        <v>276.35000000000002</v>
       </c>
       <c r="F61" s="1">
-        <v>277.37</v>
+        <v>279.14</v>
       </c>
       <c r="G61" s="1">
-        <v>274.39</v>
+        <v>281.24</v>
       </c>
       <c r="H61" s="1">
-        <v>266.54000000000002</v>
+        <v>273.45999999999998</v>
       </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
@@ -3060,28 +3060,28 @@
     </row>
     <row r="62" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="2">
-        <v>43500</v>
+        <v>43507</v>
       </c>
       <c r="B62" s="2">
-        <v>43504</v>
+        <v>43511</v>
       </c>
       <c r="C62" s="1">
-        <v>270.11</v>
+        <v>271.2</v>
       </c>
       <c r="D62" s="1">
-        <v>273.44</v>
+        <v>277.41000000000003</v>
       </c>
       <c r="E62" s="1">
-        <v>267.83</v>
+        <v>270.02999999999997</v>
       </c>
       <c r="F62" s="1">
-        <v>270.47000000000003</v>
+        <v>277.37</v>
       </c>
       <c r="G62" s="1">
-        <v>273.17</v>
+        <v>274.39</v>
       </c>
       <c r="H62" s="1">
-        <v>266.98</v>
+        <v>266.54000000000002</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
@@ -3105,28 +3105,28 @@
     </row>
     <row r="63" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="2">
-        <v>43493</v>
+        <v>43500</v>
       </c>
       <c r="B63" s="2">
-        <v>43497</v>
+        <v>43504</v>
       </c>
       <c r="C63" s="1">
-        <v>263.39</v>
+        <v>270.11</v>
       </c>
       <c r="D63" s="1">
-        <v>271.2</v>
+        <v>273.44</v>
       </c>
       <c r="E63" s="1">
-        <v>261.79000000000002</v>
+        <v>267.83</v>
       </c>
       <c r="F63" s="1">
-        <v>270.06</v>
+        <v>270.47000000000003</v>
       </c>
       <c r="G63" s="1">
-        <v>269.27999999999997</v>
+        <v>273.17</v>
       </c>
       <c r="H63" s="1">
-        <v>262.08</v>
+        <v>266.98</v>
       </c>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
@@ -3150,28 +3150,28 @@
     </row>
     <row r="64" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="2">
-        <v>43487</v>
+        <v>43493</v>
       </c>
       <c r="B64" s="2">
-        <v>43490</v>
+        <v>43497</v>
       </c>
       <c r="C64" s="1">
-        <v>264.82</v>
+        <v>263.39</v>
       </c>
       <c r="D64" s="1">
-        <v>266.7</v>
+        <v>271.2</v>
       </c>
       <c r="E64" s="1">
-        <v>260.66000000000003</v>
+        <v>261.79000000000002</v>
       </c>
       <c r="F64" s="1">
-        <v>265.77999999999997</v>
+        <v>270.06</v>
       </c>
       <c r="G64" s="1">
-        <v>270.58</v>
+        <v>269.27999999999997</v>
       </c>
       <c r="H64" s="1">
-        <v>262.18</v>
+        <v>262.08</v>
       </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
@@ -3195,28 +3195,28 @@
     </row>
     <row r="65" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="2">
-        <v>43479</v>
+        <v>43487</v>
       </c>
       <c r="B65" s="2">
-        <v>43483</v>
+        <v>43490</v>
       </c>
       <c r="C65" s="1">
-        <v>256.86</v>
+        <v>264.82</v>
       </c>
       <c r="D65" s="1">
-        <v>266.98</v>
+        <v>266.7</v>
       </c>
       <c r="E65" s="1">
-        <v>256.41000000000003</v>
+        <v>260.66000000000003</v>
       </c>
       <c r="F65" s="1">
-        <v>266.45999999999998</v>
+        <v>265.77999999999997</v>
       </c>
       <c r="G65" s="1">
-        <v>263.19</v>
+        <v>270.58</v>
       </c>
       <c r="H65" s="1">
-        <v>254.6</v>
+        <v>262.18</v>
       </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
@@ -3240,28 +3240,28 @@
     </row>
     <row r="66" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="2">
-        <v>43472</v>
+        <v>43479</v>
       </c>
       <c r="B66" s="2">
-        <v>43476</v>
+        <v>43483</v>
       </c>
       <c r="C66" s="1">
-        <v>252.69</v>
+        <v>256.86</v>
       </c>
       <c r="D66" s="1">
-        <v>259.16000000000003</v>
+        <v>266.98</v>
       </c>
       <c r="E66" s="1">
-        <v>251.69</v>
+        <v>256.41000000000003</v>
       </c>
       <c r="F66" s="1">
-        <v>258.98</v>
+        <v>266.45999999999998</v>
       </c>
       <c r="G66" s="1">
-        <v>256.42</v>
+        <v>263.19</v>
       </c>
       <c r="H66" s="1">
-        <v>248.22</v>
+        <v>254.6</v>
       </c>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
@@ -3285,28 +3285,28 @@
     </row>
     <row r="67" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="2">
-        <v>43465</v>
+        <v>43472</v>
       </c>
       <c r="B67" s="2">
-        <v>43469</v>
+        <v>43476</v>
       </c>
       <c r="C67" s="1">
-        <v>249.56</v>
+        <v>252.69</v>
       </c>
       <c r="D67" s="1">
-        <v>253.11</v>
+        <v>259.16000000000003</v>
       </c>
       <c r="E67" s="1">
-        <v>243.67</v>
+        <v>251.69</v>
       </c>
       <c r="F67" s="1">
-        <v>252.39</v>
+        <v>258.98</v>
       </c>
       <c r="G67" s="1">
-        <v>253.59</v>
+        <v>256.42</v>
       </c>
       <c r="H67" s="1">
-        <v>241.95</v>
+        <v>248.22</v>
       </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
@@ -3330,28 +3330,28 @@
     </row>
     <row r="68" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="2">
-        <v>43458</v>
+        <v>43465</v>
       </c>
       <c r="B68" s="2">
-        <v>43462</v>
+        <v>43469</v>
       </c>
       <c r="C68" s="1">
-        <v>239.04</v>
+        <v>249.56</v>
       </c>
       <c r="D68" s="1">
-        <v>251.4</v>
+        <v>253.11</v>
       </c>
       <c r="E68" s="1">
-        <v>233.76</v>
+        <v>243.67</v>
       </c>
       <c r="F68" s="1">
-        <v>247.75</v>
+        <v>252.39</v>
       </c>
       <c r="G68" s="1">
-        <v>247.01</v>
+        <v>253.59</v>
       </c>
       <c r="H68" s="1">
-        <v>234.37</v>
+        <v>241.95</v>
       </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
@@ -3375,28 +3375,28 @@
     </row>
     <row r="69" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="2">
-        <v>43451</v>
+        <v>43458</v>
       </c>
       <c r="B69" s="2">
-        <v>43455</v>
+        <v>43462</v>
       </c>
       <c r="C69" s="1">
-        <v>259.39999999999998</v>
+        <v>239.04</v>
       </c>
       <c r="D69" s="1">
-        <v>260.64999999999998</v>
+        <v>251.4</v>
       </c>
       <c r="E69" s="1">
-        <v>239.98</v>
+        <v>233.76</v>
       </c>
       <c r="F69" s="1">
-        <v>240.7</v>
+        <v>247.75</v>
       </c>
       <c r="G69" s="1">
-        <v>266.63</v>
+        <v>247.01</v>
       </c>
       <c r="H69" s="1">
-        <v>254.29</v>
+        <v>234.37</v>
       </c>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
@@ -3418,6 +3418,51 @@
       <c r="Z69" s="1"/>
       <c r="AA69" s="1"/>
     </row>
+    <row r="70" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="2">
+        <v>43451</v>
+      </c>
+      <c r="B70" s="2">
+        <v>43455</v>
+      </c>
+      <c r="C70" s="1">
+        <v>259.39999999999998</v>
+      </c>
+      <c r="D70" s="1">
+        <v>260.64999999999998</v>
+      </c>
+      <c r="E70" s="1">
+        <v>239.98</v>
+      </c>
+      <c r="F70" s="1">
+        <v>240.7</v>
+      </c>
+      <c r="G70" s="1">
+        <v>266.63</v>
+      </c>
+      <c r="H70" s="1">
+        <v>254.29</v>
+      </c>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+      <c r="Y70" s="1"/>
+      <c r="Z70" s="1"/>
+      <c r="AA70" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>